<commit_message>
The calculation engine has been corrected, H , S  and Cp can now be shown in their respective columns
</commit_message>
<xml_diff>
--- a/data_from_calculation.xlsx
+++ b/data_from_calculation.xlsx
@@ -465,16 +465,16 @@
         <v>298</v>
       </c>
       <c r="B2" t="n">
-        <v>483.654</v>
+        <v>0.1888</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08889999999999992</v>
+        <v>0.1888</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>457.1618</v>
+        <v>-298.0894</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         <v>315.1919191919192</v>
       </c>
       <c r="B3" t="n">
-        <v>483.654</v>
+        <v>433.5528</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08889999999999992</v>
+        <v>1.591382538080918</v>
       </c>
       <c r="D3" t="n">
-        <v>13.72585462707885</v>
+        <v>55.33559557188033</v>
       </c>
       <c r="E3" t="n">
-        <v>455.6334383838384</v>
+        <v>-301.3514190986176</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>332.3838383838384</v>
       </c>
       <c r="B4" t="n">
-        <v>483.654</v>
+        <v>1820.8769</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08889999999999992</v>
+        <v>5.874233231187395</v>
       </c>
       <c r="D4" t="n">
-        <v>28.19061446791145</v>
+        <v>113.7450368329763</v>
       </c>
       <c r="E4" t="n">
-        <v>454.1050767676768</v>
+        <v>-304.6447514575424</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +516,16 @@
         <v>349.5757575757576</v>
       </c>
       <c r="B5" t="n">
-        <v>483.654</v>
+        <v>4213.256300000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08889999999999992</v>
+        <v>12.89951472824541</v>
       </c>
       <c r="D5" t="n">
-        <v>43.39427952249769</v>
+        <v>175.2283237832874</v>
       </c>
       <c r="E5" t="n">
-        <v>452.5767151515152</v>
+        <v>-307.9679351065716</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         <v>366.7676767676768</v>
       </c>
       <c r="B6" t="n">
-        <v>483.654</v>
+        <v>7661.786200000001</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08889999999999992</v>
+        <v>22.54909676361415</v>
       </c>
       <c r="D6" t="n">
-        <v>59.33684979083769</v>
+        <v>239.7854564228141</v>
       </c>
       <c r="E6" t="n">
-        <v>451.0483535353536</v>
+        <v>-311.3196520566958</v>
       </c>
     </row>
     <row r="7">
@@ -550,16 +550,16 @@
         <v>383.959595959596</v>
       </c>
       <c r="B7" t="n">
-        <v>483.654</v>
+        <v>12217.5618</v>
       </c>
       <c r="C7" t="n">
-        <v>0.08889999999999992</v>
+        <v>34.72096965075368</v>
       </c>
       <c r="D7" t="n">
-        <v>76.01832527293132</v>
+        <v>307.4164347515559</v>
       </c>
       <c r="E7" t="n">
-        <v>449.519991919192</v>
+        <v>-314.6987080210346</v>
       </c>
     </row>
     <row r="8">
@@ -567,16 +567,16 @@
         <v>401.1515151515151</v>
       </c>
       <c r="B8" t="n">
-        <v>483.654</v>
+        <v>18304.9677</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08889999999999992</v>
+        <v>50.25966178108935</v>
       </c>
       <c r="D8" t="n">
-        <v>93.43870596877866</v>
+        <v>378.1212587695131</v>
       </c>
       <c r="E8" t="n">
-        <v>447.9916303030303</v>
+        <v>-318.1040157744948</v>
       </c>
     </row>
     <row r="9">
@@ -584,16 +584,16 @@
         <v>418.3434343434343</v>
       </c>
       <c r="B9" t="n">
-        <v>483.654</v>
+        <v>25301.25480000001</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08889999999999992</v>
+        <v>67.35750295331408</v>
       </c>
       <c r="D9" t="n">
-        <v>111.5979918783797</v>
+        <v>451.8999284766858</v>
       </c>
       <c r="E9" t="n">
-        <v>446.4632686868687</v>
+        <v>-321.5345813708178</v>
       </c>
     </row>
     <row r="10">
@@ -601,16 +601,16 @@
         <v>435.5353535353535</v>
       </c>
       <c r="B10" t="n">
-        <v>483.654</v>
+        <v>33561.07880000002</v>
       </c>
       <c r="C10" t="n">
-        <v>0.08889999999999992</v>
+        <v>86.73929589459027</v>
       </c>
       <c r="D10" t="n">
-        <v>130.4961830017345</v>
+        <v>528.7524438730742</v>
       </c>
       <c r="E10" t="n">
-        <v>444.9349070707071</v>
+        <v>-324.9894926287783</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         <v>452.7272727272727</v>
       </c>
       <c r="B11" t="n">
-        <v>483.654</v>
+        <v>43135.53490000001</v>
       </c>
       <c r="C11" t="n">
-        <v>0.08889999999999992</v>
+        <v>108.3450647411271</v>
       </c>
       <c r="D11" t="n">
-        <v>150.133279338843</v>
+        <v>608.6788049586778</v>
       </c>
       <c r="E11" t="n">
-        <v>443.4065454545455</v>
+        <v>-328.4679094388993</v>
       </c>
     </row>
     <row r="12">
@@ -635,16 +635,16 @@
         <v>469.9191919191919</v>
       </c>
       <c r="B12" t="n">
-        <v>483.654</v>
+        <v>54075.7183</v>
       </c>
       <c r="C12" t="n">
-        <v>0.08889999999999992</v>
+        <v>132.1214863281589</v>
       </c>
       <c r="D12" t="n">
-        <v>170.5092808897051</v>
+        <v>691.6790117334966</v>
       </c>
       <c r="E12" t="n">
-        <v>441.8781838383838</v>
+        <v>-331.9690555444687</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +652,16 @@
         <v>487.1111111111111</v>
       </c>
       <c r="B13" t="n">
-        <v>483.654</v>
+        <v>67204.82140000002</v>
       </c>
       <c r="C13" t="n">
-        <v>0.08889999999999992</v>
+        <v>159.6096186227319</v>
       </c>
       <c r="D13" t="n">
-        <v>191.624187654321</v>
+        <v>777.7530641975306</v>
       </c>
       <c r="E13" t="n">
-        <v>440.3498222222223</v>
+        <v>-335.4922115267717</v>
       </c>
     </row>
     <row r="14">
@@ -669,16 +669,16 @@
         <v>504.3030303030303</v>
       </c>
       <c r="B14" t="n">
-        <v>483.654</v>
+        <v>81117.68430000002</v>
       </c>
       <c r="C14" t="n">
-        <v>0.08889999999999992</v>
+        <v>187.7105424581645</v>
       </c>
       <c r="D14" t="n">
-        <v>213.4779996326905</v>
+        <v>866.9009623507802</v>
       </c>
       <c r="E14" t="n">
-        <v>438.8214606060607</v>
+        <v>-339.0367087817384</v>
       </c>
     </row>
     <row r="15">
@@ -686,16 +686,16 @@
         <v>521.4949494949494</v>
       </c>
       <c r="B15" t="n">
-        <v>483.654</v>
+        <v>96552.56570000004</v>
       </c>
       <c r="C15" t="n">
-        <v>0.08889999999999992</v>
+        <v>217.8512202027264</v>
       </c>
       <c r="D15" t="n">
-        <v>236.0707168248137</v>
+        <v>959.1227061932452</v>
       </c>
       <c r="E15" t="n">
-        <v>437.293098989899</v>
+        <v>-342.6019243188067</v>
       </c>
     </row>
     <row r="16">
@@ -703,16 +703,16 @@
         <v>538.6868686868686</v>
       </c>
       <c r="B16" t="n">
-        <v>483.654</v>
+        <v>113560.5608</v>
       </c>
       <c r="C16" t="n">
-        <v>0.08889999999999992</v>
+        <v>249.9971314577375</v>
       </c>
       <c r="D16" t="n">
-        <v>259.4023392306906</v>
+        <v>1054.418295724926</v>
       </c>
       <c r="E16" t="n">
-        <v>435.7647373737374</v>
+        <v>-346.1872762463059</v>
       </c>
     </row>
     <row r="17">
@@ -720,16 +720,16 @@
         <v>555.8787878787879</v>
       </c>
       <c r="B17" t="n">
-        <v>483.654</v>
+        <v>132192.7648</v>
       </c>
       <c r="C17" t="n">
-        <v>0.08889999999999992</v>
+        <v>284.1169813482944</v>
       </c>
       <c r="D17" t="n">
-        <v>283.4728668503214</v>
+        <v>1152.787730945822</v>
       </c>
       <c r="E17" t="n">
-        <v>434.2363757575758</v>
+        <v>-349.7922198336929</v>
       </c>
     </row>
     <row r="18">
@@ -737,16 +737,16 @@
         <v>573.070707070707</v>
       </c>
       <c r="B18" t="n">
-        <v>483.654</v>
+        <v>153748.0963</v>
       </c>
       <c r="C18" t="n">
-        <v>0.08889999999999992</v>
+        <v>322.3638202228148</v>
       </c>
       <c r="D18" t="n">
-        <v>308.2822996837057</v>
+        <v>1254.231011855933</v>
       </c>
       <c r="E18" t="n">
-        <v>432.7080141414142</v>
+        <v>-353.4162440613429</v>
       </c>
     </row>
     <row r="19">
@@ -754,16 +754,16 @@
         <v>590.2626262626262</v>
       </c>
       <c r="B19" t="n">
-        <v>483.654</v>
+        <v>175885.1478</v>
       </c>
       <c r="C19" t="n">
-        <v>0.08889999999999992</v>
+        <v>360.4608268410215</v>
       </c>
       <c r="D19" t="n">
-        <v>333.8306377308437</v>
+        <v>1358.748138455259</v>
       </c>
       <c r="E19" t="n">
-        <v>431.1796525252525</v>
+        <v>-357.0588685846923</v>
       </c>
     </row>
     <row r="20">
@@ -771,16 +771,16 @@
         <v>607.4545454545455</v>
       </c>
       <c r="B20" t="n">
-        <v>483.654</v>
+        <v>199802.6994</v>
       </c>
       <c r="C20" t="n">
-        <v>0.08889999999999992</v>
+        <v>400.4522864453961</v>
       </c>
       <c r="D20" t="n">
-        <v>360.1178809917356</v>
+        <v>1466.339110743802</v>
       </c>
       <c r="E20" t="n">
-        <v>429.651290909091</v>
+        <v>-360.7196410523359</v>
       </c>
     </row>
     <row r="21">
@@ -788,16 +788,16 @@
         <v>624.6464646464647</v>
       </c>
       <c r="B21" t="n">
-        <v>483.654</v>
+        <v>225551.8462999999</v>
       </c>
       <c r="C21" t="n">
-        <v>0.08889999999999992</v>
+        <v>442.3165424336379</v>
       </c>
       <c r="D21" t="n">
-        <v>387.144029466381</v>
+        <v>1577.003928721559</v>
       </c>
       <c r="E21" t="n">
-        <v>428.1229292929293</v>
+        <v>-364.3981347279474</v>
       </c>
     </row>
     <row r="22">
@@ -805,16 +805,16 @@
         <v>641.8383838383838</v>
       </c>
       <c r="B22" t="n">
-        <v>483.654</v>
+        <v>253183.6836999999</v>
       </c>
       <c r="C22" t="n">
-        <v>0.08889999999999992</v>
+        <v>486.0336862472122</v>
       </c>
       <c r="D22" t="n">
-        <v>414.9090831547801</v>
+        <v>1690.742592388532</v>
       </c>
       <c r="E22" t="n">
-        <v>426.5945676767677</v>
+        <v>-368.0939463741797</v>
       </c>
     </row>
     <row r="23">
@@ -822,16 +822,16 @@
         <v>659.030303030303</v>
       </c>
       <c r="B23" t="n">
-        <v>483.654</v>
+        <v>284549.7747999997</v>
       </c>
       <c r="C23" t="n">
-        <v>0.08889999999999992</v>
+        <v>534.3216477183778</v>
       </c>
       <c r="D23" t="n">
-        <v>443.413042056933</v>
+        <v>1807.55510174472</v>
       </c>
       <c r="E23" t="n">
-        <v>425.0662060606061</v>
+        <v>-371.8066943634312</v>
       </c>
     </row>
     <row r="24">
@@ -839,16 +839,16 @@
         <v>676.2222222222222</v>
       </c>
       <c r="B24" t="n">
-        <v>483.654</v>
+        <v>316218.6276999998</v>
       </c>
       <c r="C24" t="n">
-        <v>0.08889999999999992</v>
+        <v>581.797359174214</v>
       </c>
       <c r="D24" t="n">
-        <v>472.6559061728394</v>
+        <v>1927.441456790123</v>
       </c>
       <c r="E24" t="n">
-        <v>423.5378444444445</v>
+        <v>-375.536016985866</v>
       </c>
     </row>
     <row r="25">
@@ -856,16 +856,16 @@
         <v>693.4141414141413</v>
       </c>
       <c r="B25" t="n">
-        <v>483.654</v>
+        <v>349926.4622999997</v>
       </c>
       <c r="C25" t="n">
-        <v>0.08889999999999992</v>
+        <v>631.0741171244933</v>
       </c>
       <c r="D25" t="n">
-        <v>502.6376755024996</v>
+        <v>2050.401657524742</v>
       </c>
       <c r="E25" t="n">
-        <v>422.0094828282829</v>
+        <v>-379.2815709295954</v>
       </c>
     </row>
     <row r="26">
@@ -873,16 +873,16 @@
         <v>710.6060606060605</v>
       </c>
       <c r="B26" t="n">
-        <v>483.654</v>
+        <v>385724.3737999996</v>
       </c>
       <c r="C26" t="n">
-        <v>0.08889999999999992</v>
+        <v>682.1374538026547</v>
       </c>
       <c r="D26" t="n">
-        <v>533.3583500459135</v>
+        <v>2176.435703948576</v>
       </c>
       <c r="E26" t="n">
-        <v>420.4811212121213</v>
+        <v>-383.0430299116661</v>
       </c>
     </row>
     <row r="27">
@@ -890,16 +890,16 @@
         <v>727.7979797979797</v>
       </c>
       <c r="B27" t="n">
-        <v>483.654</v>
+        <v>423663.4573999995</v>
       </c>
       <c r="C27" t="n">
-        <v>0.08889999999999992</v>
+        <v>734.9739292954573</v>
       </c>
       <c r="D27" t="n">
-        <v>564.8179298030811</v>
+        <v>2305.543596061626</v>
       </c>
       <c r="E27" t="n">
-        <v>418.9527595959597</v>
+        <v>-386.8200834415991</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +907,16 @@
         <v>744.989898989899</v>
       </c>
       <c r="B28" t="n">
-        <v>483.654</v>
+        <v>463794.8082999997</v>
       </c>
       <c r="C28" t="n">
-        <v>0.08889999999999992</v>
+        <v>789.5710364268923</v>
       </c>
       <c r="D28" t="n">
-        <v>597.0164147740027</v>
+        <v>2437.725333863891</v>
       </c>
       <c r="E28" t="n">
-        <v>417.424397979798</v>
+        <v>-390.6124357018165</v>
       </c>
     </row>
     <row r="29">
@@ -924,16 +924,16 @@
         <v>762.1818181818181</v>
       </c>
       <c r="B29" t="n">
-        <v>483.654</v>
+        <v>508733.1063999996</v>
       </c>
       <c r="C29" t="n">
-        <v>0.08889999999999992</v>
+        <v>849.2858216523955</v>
       </c>
       <c r="D29" t="n">
-        <v>629.9538049586777</v>
+        <v>2572.980917355371</v>
       </c>
       <c r="E29" t="n">
-        <v>415.8960363636364</v>
+        <v>-394.4198045314602</v>
       </c>
     </row>
     <row r="30">
@@ -941,16 +941,16 @@
         <v>779.3737373737373</v>
       </c>
       <c r="B30" t="n">
-        <v>483.654</v>
+        <v>553538.8367999995</v>
       </c>
       <c r="C30" t="n">
-        <v>0.08889999999999992</v>
+        <v>907.4719058507873</v>
       </c>
       <c r="D30" t="n">
-        <v>663.6301003571062</v>
+        <v>2711.310346536067</v>
       </c>
       <c r="E30" t="n">
-        <v>414.3676747474748</v>
+        <v>-398.2419205019363</v>
       </c>
     </row>
     <row r="31">
@@ -958,16 +958,16 @@
         <v>796.5656565656566</v>
       </c>
       <c r="B31" t="n">
-        <v>483.654</v>
+        <v>600693.1256999994</v>
       </c>
       <c r="C31" t="n">
-        <v>0.08889999999999992</v>
+        <v>967.3853203089856</v>
       </c>
       <c r="D31" t="n">
-        <v>698.0453009692889</v>
+        <v>2852.713621405979</v>
       </c>
       <c r="E31" t="n">
-        <v>412.8393131313132</v>
+        <v>-402.0785260740635</v>
       </c>
     </row>
     <row r="32">
@@ -975,16 +975,16 @@
         <v>813.7575757575758</v>
       </c>
       <c r="B32" t="n">
-        <v>483.654</v>
+        <v>650247.0682999993</v>
       </c>
       <c r="C32" t="n">
-        <v>0.08889999999999992</v>
+        <v>1029.016568885356</v>
       </c>
       <c r="D32" t="n">
-        <v>733.1994067952251</v>
+        <v>2997.190741965106</v>
       </c>
       <c r="E32" t="n">
-        <v>411.3109515151516</v>
+        <v>-405.9293748280133</v>
       </c>
     </row>
     <row r="33">
@@ -992,16 +992,16 @@
         <v>830.9494949494949</v>
       </c>
       <c r="B33" t="n">
-        <v>483.654</v>
+        <v>702251.7597999993</v>
       </c>
       <c r="C33" t="n">
-        <v>0.08889999999999992</v>
+        <v>1092.356745419338</v>
       </c>
       <c r="D33" t="n">
-        <v>769.0924178349148</v>
+        <v>3144.741708213448</v>
       </c>
       <c r="E33" t="n">
-        <v>409.78258989899</v>
+        <v>-409.7942307583525</v>
       </c>
     </row>
     <row r="34">
@@ -1009,16 +1009,16 @@
         <v>848.1414141414141</v>
       </c>
       <c r="B34" t="n">
-        <v>483.654</v>
+        <v>760043.5662999992</v>
       </c>
       <c r="C34" t="n">
-        <v>0.08889999999999992</v>
+        <v>1161.276200016197</v>
       </c>
       <c r="D34" t="n">
-        <v>805.7243340883582</v>
+        <v>3295.366520151004</v>
       </c>
       <c r="E34" t="n">
-        <v>408.2542282828284</v>
+        <v>-413.672867627446</v>
       </c>
     </row>
     <row r="35">
@@ -1026,16 +1026,16 @@
         <v>865.3333333333333</v>
       </c>
       <c r="B35" t="n">
-        <v>483.654</v>
+        <v>817254.8052999993</v>
       </c>
       <c r="C35" t="n">
-        <v>0.08889999999999992</v>
+        <v>1228.108974855672</v>
       </c>
       <c r="D35" t="n">
-        <v>843.0951555555554</v>
+        <v>3449.065177777777</v>
       </c>
       <c r="E35" t="n">
-        <v>406.7258666666667</v>
+        <v>-417.5650683713066</v>
       </c>
     </row>
     <row r="36">
@@ -1043,16 +1043,16 @@
         <v>882.5252525252524</v>
       </c>
       <c r="B36" t="n">
-        <v>483.654</v>
+        <v>877073.0843999991</v>
       </c>
       <c r="C36" t="n">
-        <v>0.08889999999999992</v>
+        <v>1296.626621445597</v>
       </c>
       <c r="D36" t="n">
-        <v>881.2048822365064</v>
+        <v>3605.837681093765</v>
       </c>
       <c r="E36" t="n">
-        <v>405.1975050505051</v>
+        <v>-421.4706245526768</v>
       </c>
     </row>
     <row r="37">
@@ -1060,16 +1060,16 @@
         <v>899.7171717171717</v>
       </c>
       <c r="B37" t="n">
-        <v>483.654</v>
+        <v>939549.4987999991</v>
       </c>
       <c r="C37" t="n">
-        <v>0.08889999999999992</v>
+        <v>1366.822183591178</v>
       </c>
       <c r="D37" t="n">
-        <v>920.0535141312112</v>
+        <v>3765.684030098969</v>
       </c>
       <c r="E37" t="n">
-        <v>403.6691434343435</v>
+        <v>-425.3893358567419</v>
       </c>
     </row>
     <row r="38">
@@ -1077,16 +1077,16 @@
         <v>916.9090909090909</v>
       </c>
       <c r="B38" t="n">
-        <v>483.654</v>
+        <v>1004735.143699999</v>
       </c>
       <c r="C38" t="n">
-        <v>0.08889999999999992</v>
+        <v>1438.689096286766</v>
       </c>
       <c r="D38" t="n">
-        <v>959.6410512396694</v>
+        <v>3928.604224793388</v>
       </c>
       <c r="E38" t="n">
-        <v>402.1407818181819</v>
+        <v>-429.3210096253982</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         <v>934.10101010101</v>
       </c>
       <c r="B39" t="n">
-        <v>483.654</v>
+        <v>1076764.989799999</v>
       </c>
       <c r="C39" t="n">
-        <v>0.08889999999999992</v>
+        <v>1516.598301081473</v>
       </c>
       <c r="D39" t="n">
-        <v>999.9674935618814</v>
+        <v>4094.598265177022</v>
       </c>
       <c r="E39" t="n">
-        <v>400.6124202020203</v>
+        <v>-433.2654604264631</v>
       </c>
     </row>
     <row r="40">
@@ -1111,16 +1111,16 @@
         <v>951.2929292929292</v>
       </c>
       <c r="B40" t="n">
-        <v>483.654</v>
+        <v>1147689.350199999</v>
       </c>
       <c r="C40" t="n">
-        <v>0.08889999999999992</v>
+        <v>1591.887072146943</v>
       </c>
       <c r="D40" t="n">
-        <v>1041.032841097847</v>
+        <v>4263.666151249871</v>
       </c>
       <c r="E40" t="n">
-        <v>399.0840585858587</v>
+        <v>-437.2225096546076</v>
       </c>
     </row>
     <row r="41">
@@ -1128,16 +1128,16 @@
         <v>968.4848484848484</v>
       </c>
       <c r="B41" t="n">
-        <v>483.654</v>
+        <v>1221479.232299999</v>
       </c>
       <c r="C41" t="n">
-        <v>0.08889999999999992</v>
+        <v>1668.82925322115</v>
       </c>
       <c r="D41" t="n">
-        <v>1082.837093847566</v>
+        <v>4435.807883011936</v>
       </c>
       <c r="E41" t="n">
-        <v>397.5556969696971</v>
+        <v>-441.1919851611453</v>
       </c>
     </row>
     <row r="42">
@@ -1145,16 +1145,16 @@
         <v>985.6767676767677</v>
       </c>
       <c r="B42" t="n">
-        <v>483.654</v>
+        <v>1298185.731299999</v>
       </c>
       <c r="C42" t="n">
-        <v>0.08889999999999992</v>
+        <v>1747.419597240242</v>
       </c>
       <c r="D42" t="n">
-        <v>1125.38025181104</v>
+        <v>4611.023460463218</v>
       </c>
       <c r="E42" t="n">
-        <v>396.0273353535354</v>
+        <v>-445.1737209101161</v>
       </c>
     </row>
     <row r="43">
@@ -1162,16 +1162,16 @@
         <v>1002.868686868687</v>
       </c>
       <c r="B43" t="n">
-        <v>483.654</v>
+        <v>1377859.942399999</v>
       </c>
       <c r="C43" t="n">
-        <v>0.08889999999999992</v>
+        <v>1827.653126653972</v>
       </c>
       <c r="D43" t="n">
-        <v>1168.662314988266</v>
+        <v>4789.312883603713</v>
       </c>
       <c r="E43" t="n">
-        <v>394.4989737373738</v>
+        <v>-449.1675566583691</v>
       </c>
     </row>
     <row r="44">
@@ -1179,16 +1179,16 @@
         <v>1020.060606060606</v>
       </c>
       <c r="B44" t="n">
-        <v>483.654</v>
+        <v>1465512.359299999</v>
       </c>
       <c r="C44" t="n">
-        <v>0.08889999999999992</v>
+        <v>1914.392042167121</v>
       </c>
       <c r="D44" t="n">
-        <v>1212.683283379247</v>
+        <v>4970.676152433424</v>
       </c>
       <c r="E44" t="n">
-        <v>392.9706121212122</v>
+        <v>-453.1733376575895</v>
       </c>
     </row>
     <row r="45">
@@ -1196,16 +1196,16 @@
         <v>1037.252525252525</v>
       </c>
       <c r="B45" t="n">
-        <v>483.654</v>
+        <v>1551457.453899998</v>
       </c>
       <c r="C45" t="n">
-        <v>0.08889999999999992</v>
+        <v>1997.993979177454</v>
       </c>
       <c r="D45" t="n">
-        <v>1257.443156983981</v>
+        <v>5155.113266952349</v>
       </c>
       <c r="E45" t="n">
-        <v>391.4422505050506</v>
+        <v>-457.190914376417</v>
       </c>
     </row>
     <row r="46">
@@ -1213,16 +1213,16 @@
         <v>1054.444444444444</v>
       </c>
       <c r="B46" t="n">
-        <v>483.654</v>
+        <v>1640526.551799998</v>
       </c>
       <c r="C46" t="n">
-        <v>0.08889999999999992</v>
+        <v>2083.225367131771</v>
       </c>
       <c r="D46" t="n">
-        <v>1302.941935802469</v>
+        <v>5342.624227160492</v>
       </c>
       <c r="E46" t="n">
-        <v>389.913888888889</v>
+        <v>-461.2201422409924</v>
       </c>
     </row>
     <row r="47">
@@ -1230,16 +1230,16 @@
         <v>1071.636363636364</v>
       </c>
       <c r="B47" t="n">
-        <v>483.654</v>
+        <v>1732770.748199998</v>
       </c>
       <c r="C47" t="n">
-        <v>0.08889999999999992</v>
+        <v>2170.082151028627</v>
       </c>
       <c r="D47" t="n">
-        <v>1349.179619834711</v>
+        <v>5533.209033057849</v>
       </c>
       <c r="E47" t="n">
-        <v>388.3855272727274</v>
+        <v>-465.2608813924289</v>
       </c>
     </row>
     <row r="48">
@@ -1247,16 +1247,16 @@
         <v>1088.828282828283</v>
       </c>
       <c r="B48" t="n">
-        <v>483.654</v>
+        <v>1828241.138299998</v>
       </c>
       <c r="C48" t="n">
-        <v>0.08889999999999992</v>
+        <v>2258.56046754642</v>
       </c>
       <c r="D48" t="n">
-        <v>1396.156209080706</v>
+        <v>5726.867684644422</v>
       </c>
       <c r="E48" t="n">
-        <v>386.8571656565658</v>
+        <v>-469.3129964598491</v>
       </c>
     </row>
     <row r="49">
@@ -1264,16 +1264,16 @@
         <v>1106.020202020202</v>
       </c>
       <c r="B49" t="n">
-        <v>483.654</v>
+        <v>1932900.657199998</v>
       </c>
       <c r="C49" t="n">
-        <v>0.08889999999999992</v>
+        <v>2354.006714507076</v>
       </c>
       <c r="D49" t="n">
-        <v>1443.871703540455</v>
+        <v>5923.60018192021</v>
       </c>
       <c r="E49" t="n">
-        <v>385.3288040404041</v>
+        <v>-473.3763563477611</v>
       </c>
     </row>
     <row r="50">
@@ -1281,16 +1281,16 @@
         <v>1123.212121212121</v>
       </c>
       <c r="B50" t="n">
-        <v>483.654</v>
+        <v>2035174.098799998</v>
       </c>
       <c r="C50" t="n">
-        <v>0.08889999999999992</v>
+        <v>2445.812069288779</v>
       </c>
       <c r="D50" t="n">
-        <v>1492.326103213957</v>
+        <v>6123.406524885213</v>
       </c>
       <c r="E50" t="n">
-        <v>383.8004424242425</v>
+        <v>-477.4508340366556</v>
       </c>
     </row>
     <row r="51">
@@ -1298,16 +1298,16 @@
         <v>1140.40404040404</v>
       </c>
       <c r="B51" t="n">
-        <v>483.654</v>
+        <v>2140830.025299998</v>
       </c>
       <c r="C51" t="n">
-        <v>0.08889999999999992</v>
+        <v>2539.228209646674</v>
       </c>
       <c r="D51" t="n">
-        <v>1541.519408101213</v>
+        <v>6326.286713539432</v>
       </c>
       <c r="E51" t="n">
-        <v>382.2720808080809</v>
+        <v>-481.5363063958152</v>
       </c>
     </row>
     <row r="52">
@@ -1315,16 +1315,16 @@
         <v>1157.595959595959</v>
       </c>
       <c r="B52" t="n">
-        <v>483.654</v>
+        <v>2249919.531899997</v>
       </c>
       <c r="C52" t="n">
-        <v>0.08889999999999992</v>
+        <v>2634.251937224288</v>
       </c>
       <c r="D52" t="n">
-        <v>1591.451618202223</v>
+        <v>6532.240747882865</v>
       </c>
       <c r="E52" t="n">
-        <v>380.7437191919193</v>
+        <v>-485.6326540074128</v>
       </c>
     </row>
     <row r="53">
@@ -1332,16 +1332,16 @@
         <v>1174.787878787879</v>
       </c>
       <c r="B53" t="n">
-        <v>483.654</v>
+        <v>2362493.713799998</v>
       </c>
       <c r="C53" t="n">
-        <v>0.08889999999999992</v>
+        <v>2730.880193689168</v>
       </c>
       <c r="D53" t="n">
-        <v>1642.122733516988</v>
+        <v>6741.268627915518</v>
       </c>
       <c r="E53" t="n">
-        <v>379.2153575757577</v>
+        <v>-489.7397610010625</v>
       </c>
     </row>
     <row r="54">
@@ -1349,16 +1349,16 @@
         <v>1191.979797979798</v>
       </c>
       <c r="B54" t="n">
-        <v>483.654</v>
+        <v>2478603.666199998</v>
       </c>
       <c r="C54" t="n">
-        <v>0.08889999999999992</v>
+        <v>2829.110052676634</v>
       </c>
       <c r="D54" t="n">
-        <v>1693.532754045505</v>
+        <v>6953.370353637383</v>
       </c>
       <c r="E54" t="n">
-        <v>377.6869959595961</v>
+        <v>-493.8575148980554</v>
       </c>
     </row>
     <row r="55">
@@ -1366,16 +1366,16 @@
         <v>1209.171717171717</v>
       </c>
       <c r="B55" t="n">
-        <v>483.654</v>
+        <v>2605454.267299998</v>
       </c>
       <c r="C55" t="n">
-        <v>0.08889999999999992</v>
+        <v>2934.860718099435</v>
       </c>
       <c r="D55" t="n">
-        <v>1745.681679787776</v>
+        <v>7168.545925048463</v>
       </c>
       <c r="E55" t="n">
-        <v>376.1586343434344</v>
+        <v>-497.9858064645853</v>
       </c>
     </row>
     <row r="56">
@@ -1383,16 +1383,16 @@
         <v>1226.363636363636</v>
       </c>
       <c r="B56" t="n">
-        <v>483.654</v>
+        <v>2729004.635199997</v>
       </c>
       <c r="C56" t="n">
-        <v>0.08889999999999992</v>
+        <v>3036.379302008363</v>
       </c>
       <c r="D56" t="n">
-        <v>1798.569510743801</v>
+        <v>7386.795342148758</v>
       </c>
       <c r="E56" t="n">
-        <v>374.6302727272728</v>
+        <v>-502.1245295733219</v>
       </c>
     </row>
     <row r="57">
@@ -1400,16 +1400,16 @@
         <v>1243.555555555555</v>
       </c>
       <c r="B57" t="n">
-        <v>483.654</v>
+        <v>2856247.064799997</v>
       </c>
       <c r="C57" t="n">
-        <v>0.08889999999999992</v>
+        <v>3139.491280829887</v>
       </c>
       <c r="D57" t="n">
-        <v>1852.19624691358</v>
+        <v>7608.11860493827</v>
       </c>
       <c r="E57" t="n">
-        <v>373.1019111111112</v>
+        <v>-506.2735810727474</v>
       </c>
     </row>
     <row r="58">
@@ -1417,16 +1417,16 @@
         <v>1260.747474747475</v>
       </c>
       <c r="B58" t="n">
-        <v>483.654</v>
+        <v>2987232.651299998</v>
       </c>
       <c r="C58" t="n">
-        <v>0.08889999999999992</v>
+        <v>3244.194192237297</v>
       </c>
       <c r="D58" t="n">
-        <v>1906.561888297112</v>
+        <v>7832.515713416997</v>
       </c>
       <c r="E58" t="n">
-        <v>371.5735494949496</v>
+        <v>-510.4328606637212</v>
       </c>
     </row>
     <row r="59">
@@ -1434,16 +1434,16 @@
         <v>1277.939393939394</v>
       </c>
       <c r="B59" t="n">
-        <v>483.654</v>
+        <v>3122012.489899998</v>
       </c>
       <c r="C59" t="n">
-        <v>0.08889999999999992</v>
+        <v>3350.485672946719</v>
       </c>
       <c r="D59" t="n">
-        <v>1961.666434894399</v>
+        <v>8059.986667584941</v>
       </c>
       <c r="E59" t="n">
-        <v>370.0451878787879</v>
+        <v>-514.6022707827769</v>
       </c>
     </row>
     <row r="60">
@@ -1451,16 +1451,16 @@
         <v>1295.131313131313</v>
       </c>
       <c r="B60" t="n">
-        <v>483.654</v>
+        <v>3268912.941799997</v>
       </c>
       <c r="C60" t="n">
-        <v>0.08889999999999992</v>
+        <v>3464.75855857601</v>
       </c>
       <c r="D60" t="n">
-        <v>2017.509886705438</v>
+        <v>8290.531467442099</v>
       </c>
       <c r="E60" t="n">
-        <v>368.5168262626264</v>
+        <v>-518.7817164917011</v>
       </c>
     </row>
     <row r="61">
@@ -1468,16 +1468,16 @@
         <v>1312.323232323232</v>
       </c>
       <c r="B61" t="n">
-        <v>483.654</v>
+        <v>3411665.363899997</v>
       </c>
       <c r="C61" t="n">
-        <v>0.08889999999999992</v>
+        <v>3574.313575744999</v>
       </c>
       <c r="D61" t="n">
-        <v>2074.092243730232</v>
+        <v>8524.150112988471</v>
       </c>
       <c r="E61" t="n">
-        <v>366.9884646464648</v>
+        <v>-522.9711053729759</v>
       </c>
     </row>
     <row r="62">
@@ -1485,16 +1485,16 @@
         <v>1329.515151515152</v>
       </c>
       <c r="B62" t="n">
-        <v>483.654</v>
+        <v>3558368.329299998</v>
       </c>
       <c r="C62" t="n">
-        <v>0.08889999999999992</v>
+        <v>3685.450495113501</v>
       </c>
       <c r="D62" t="n">
-        <v>2131.413505968779</v>
+        <v>8760.842604224057</v>
       </c>
       <c r="E62" t="n">
-        <v>365.4601030303031</v>
+        <v>-527.1703474307013</v>
       </c>
     </row>
     <row r="63">
@@ -1502,16 +1502,16 @@
         <v>1346.707070707071</v>
       </c>
       <c r="B63" t="n">
-        <v>483.654</v>
+        <v>3709072.933199999</v>
       </c>
       <c r="C63" t="n">
-        <v>0.08889999999999992</v>
+        <v>3798.167305025181</v>
       </c>
       <c r="D63" t="n">
-        <v>2189.47367342108</v>
+        <v>9000.608941148863</v>
       </c>
       <c r="E63" t="n">
-        <v>363.9317414141415</v>
+        <v>-531.3793549966429</v>
       </c>
     </row>
     <row r="64">
@@ -1519,16 +1519,16 @@
         <v>1363.89898989899</v>
       </c>
       <c r="B64" t="n">
-        <v>483.654</v>
+        <v>3863830.2708</v>
       </c>
       <c r="C64" t="n">
-        <v>0.08889999999999992</v>
+        <v>3912.462069599144</v>
       </c>
       <c r="D64" t="n">
-        <v>2248.272746087134</v>
+        <v>9243.449123762879</v>
       </c>
       <c r="E64" t="n">
-        <v>362.4033797979799</v>
+        <v>-535.5980426410779</v>
       </c>
     </row>
     <row r="65">
@@ -1536,16 +1536,16 @@
         <v>1381.090909090909</v>
       </c>
       <c r="B65" t="n">
-        <v>483.654</v>
+        <v>4032165.1047</v>
       </c>
       <c r="C65" t="n">
-        <v>0.08889999999999992</v>
+        <v>4035.197901348132</v>
       </c>
       <c r="D65" t="n">
-        <v>2307.810723966942</v>
+        <v>9489.363152066115</v>
       </c>
       <c r="E65" t="n">
-        <v>360.8750181818183</v>
+        <v>-539.8263270881364</v>
       </c>
     </row>
     <row r="66">
@@ -1553,16 +1553,16 @@
         <v>1398.282828282828</v>
       </c>
       <c r="B66" t="n">
-        <v>483.654</v>
+        <v>4195427.193799999</v>
       </c>
       <c r="C66" t="n">
-        <v>0.08889999999999992</v>
+        <v>4152.735603253509</v>
       </c>
       <c r="D66" t="n">
-        <v>2368.087607060504</v>
+        <v>9738.351026058563</v>
       </c>
       <c r="E66" t="n">
-        <v>359.3466565656566</v>
+        <v>-544.0641271353594</v>
       </c>
     </row>
     <row r="67">
@@ -1570,16 +1570,16 @@
         <v>1415.474747474747</v>
       </c>
       <c r="B67" t="n">
-        <v>483.654</v>
+        <v>4362898.307799999</v>
       </c>
       <c r="C67" t="n">
-        <v>0.08889999999999992</v>
+        <v>4271.845770564658</v>
       </c>
       <c r="D67" t="n">
-        <v>2429.103395367819</v>
+        <v>9990.412745740228</v>
       </c>
       <c r="E67" t="n">
-        <v>357.8182949494951</v>
+        <v>-548.3113635772131</v>
       </c>
     </row>
     <row r="68">
@@ -1587,16 +1587,16 @@
         <v>1432.666666666667</v>
       </c>
       <c r="B68" t="n">
-        <v>483.654</v>
+        <v>4534629.5419</v>
       </c>
       <c r="C68" t="n">
-        <v>0.08889999999999992</v>
+        <v>4392.526738693349</v>
       </c>
       <c r="D68" t="n">
-        <v>2490.858088888888</v>
+        <v>10245.54831111111</v>
       </c>
       <c r="E68" t="n">
-        <v>356.2899333333335</v>
+        <v>-552.5679591323191</v>
       </c>
     </row>
     <row r="69">
@@ -1604,16 +1604,16 @@
         <v>1449.858585858586</v>
       </c>
       <c r="B69" t="n">
-        <v>483.654</v>
+        <v>4710671.9913</v>
       </c>
       <c r="C69" t="n">
-        <v>0.08889999999999992</v>
+        <v>4514.776902008308</v>
       </c>
       <c r="D69" t="n">
-        <v>2553.351687623711</v>
+        <v>10503.7577221712</v>
       </c>
       <c r="E69" t="n">
-        <v>354.7615717171718</v>
+        <v>-556.8338383741783</v>
       </c>
     </row>
     <row r="70">
@@ -1621,16 +1621,16 @@
         <v>1467.050505050505</v>
       </c>
       <c r="B70" t="n">
-        <v>483.654</v>
+        <v>4901825.7384</v>
       </c>
       <c r="C70" t="n">
-        <v>0.08889999999999992</v>
+        <v>4645.926898805133</v>
       </c>
       <c r="D70" t="n">
-        <v>2616.584191572288</v>
+        <v>10765.04097892052</v>
       </c>
       <c r="E70" t="n">
-        <v>353.2332101010102</v>
+        <v>-561.1089276651819</v>
       </c>
     </row>
     <row r="71">
@@ -1638,16 +1638,16 @@
         <v>1484.242424242424</v>
       </c>
       <c r="B71" t="n">
-        <v>483.654</v>
+        <v>5086905.107299997</v>
       </c>
       <c r="C71" t="n">
-        <v>0.08889999999999992</v>
+        <v>4771.402938816865</v>
       </c>
       <c r="D71" t="n">
-        <v>2680.555600734618</v>
+        <v>11029.39808135904</v>
       </c>
       <c r="E71" t="n">
-        <v>351.7048484848486</v>
+        <v>-565.3931550937141</v>
       </c>
     </row>
     <row r="72">
@@ -1655,16 +1655,16 @@
         <v>1501.434343434343</v>
       </c>
       <c r="B72" t="n">
-        <v>483.654</v>
+        <v>5276451.982699999</v>
       </c>
       <c r="C72" t="n">
-        <v>0.08889999999999992</v>
+        <v>4898.44360069199</v>
       </c>
       <c r="D72" t="n">
-        <v>2745.265915110703</v>
+        <v>11296.82902948679</v>
       </c>
       <c r="E72" t="n">
-        <v>350.176486868687</v>
+        <v>-569.686450414171</v>
       </c>
     </row>
     <row r="73">
@@ -1672,16 +1672,16 @@
         <v>1518.626262626263</v>
       </c>
       <c r="B73" t="n">
-        <v>483.654</v>
+        <v>5470517.459799997</v>
       </c>
       <c r="C73" t="n">
-        <v>0.08889999999999992</v>
+        <v>5027.047491448012</v>
       </c>
       <c r="D73" t="n">
-        <v>2810.715134700541</v>
+        <v>11567.33382330374</v>
       </c>
       <c r="E73" t="n">
-        <v>348.6481252525253</v>
+        <v>-573.9887449897259</v>
       </c>
     </row>
     <row r="74">
@@ -1689,16 +1689,16 @@
         <v>1535.818181818182</v>
       </c>
       <c r="B74" t="n">
-        <v>483.654</v>
+        <v>5669152.633799996</v>
       </c>
       <c r="C74" t="n">
-        <v>0.08889999999999992</v>
+        <v>5157.213264658852</v>
       </c>
       <c r="D74" t="n">
-        <v>2876.903259504132</v>
+        <v>11840.91246280992</v>
       </c>
       <c r="E74" t="n">
-        <v>347.1197636363638</v>
+        <v>-578.2999717376878</v>
       </c>
     </row>
     <row r="75">
@@ -1706,16 +1706,16 @@
         <v>1553.010101010101</v>
       </c>
       <c r="B75" t="n">
-        <v>483.654</v>
+        <v>5884509.825299996</v>
       </c>
       <c r="C75" t="n">
-        <v>0.08889999999999992</v>
+        <v>5296.736799717429</v>
       </c>
       <c r="D75" t="n">
-        <v>2943.830289521477</v>
+        <v>12117.5649480053</v>
       </c>
       <c r="E75" t="n">
-        <v>345.5914020202022</v>
+        <v>-582.6200650773048</v>
       </c>
     </row>
     <row r="76">
@@ -1723,16 +1723,16 @@
         <v>1570.20202020202</v>
       </c>
       <c r="B76" t="n">
-        <v>483.654</v>
+        <v>6092714.086799998</v>
       </c>
       <c r="C76" t="n">
-        <v>0.08889999999999992</v>
+        <v>5430.114161073618</v>
       </c>
       <c r="D76" t="n">
-        <v>3011.496224752576</v>
+        <v>12397.29127888991</v>
       </c>
       <c r="E76" t="n">
-        <v>344.0630404040405</v>
+        <v>-586.948960879882</v>
       </c>
     </row>
     <row r="77">
@@ -1740,16 +1740,16 @@
         <v>1587.393939393939</v>
       </c>
       <c r="B77" t="n">
-        <v>483.654</v>
+        <v>6305644.336399998</v>
       </c>
       <c r="C77" t="n">
-        <v>0.08889999999999992</v>
+        <v>5565.049554524971</v>
       </c>
       <c r="D77" t="n">
-        <v>3079.901065197429</v>
+        <v>12680.09145546373</v>
       </c>
       <c r="E77" t="n">
-        <v>342.5346787878789</v>
+        <v>-591.2865964210808</v>
       </c>
     </row>
     <row r="78">
@@ -1757,16 +1757,16 @@
         <v>1604.585858585858</v>
       </c>
       <c r="B78" t="n">
-        <v>483.654</v>
+        <v>6523351.669299998</v>
       </c>
       <c r="C78" t="n">
-        <v>0.08889999999999992</v>
+        <v>5701.541802676525</v>
       </c>
       <c r="D78" t="n">
-        <v>3149.044810856034</v>
+        <v>12965.96547772676</v>
       </c>
       <c r="E78" t="n">
-        <v>341.0063171717173</v>
+        <v>-595.632910335288</v>
       </c>
     </row>
     <row r="79">
@@ -1774,16 +1774,16 @@
         <v>1621.777777777778</v>
       </c>
       <c r="B79" t="n">
-        <v>483.654</v>
+        <v>6745887.180699999</v>
       </c>
       <c r="C79" t="n">
-        <v>0.08889999999999992</v>
+        <v>5839.58976538481</v>
       </c>
       <c r="D79" t="n">
-        <v>3218.927461728394</v>
+        <v>13254.91334567901</v>
       </c>
       <c r="E79" t="n">
-        <v>339.4779555555557</v>
+        <v>-599.9878425719377</v>
       </c>
     </row>
     <row r="80">
@@ -1791,16 +1791,16 @@
         <v>1638.969696969697</v>
       </c>
       <c r="B80" t="n">
-        <v>483.654</v>
+        <v>6973301.965799997</v>
       </c>
       <c r="C80" t="n">
-        <v>0.08889999999999992</v>
+        <v>5979.192338202761</v>
       </c>
       <c r="D80" t="n">
-        <v>3289.549017814508</v>
+        <v>13546.93505932047</v>
       </c>
       <c r="E80" t="n">
-        <v>337.949593939394</v>
+        <v>-604.3513343536889</v>
       </c>
     </row>
     <row r="81">
@@ -1808,16 +1808,16 @@
         <v>1656.161616161616</v>
       </c>
       <c r="B81" t="n">
-        <v>483.654</v>
+        <v>7219469.114699996</v>
       </c>
       <c r="C81" t="n">
-        <v>0.08889999999999992</v>
+        <v>6128.700109454816</v>
       </c>
       <c r="D81" t="n">
-        <v>3360.909479114375</v>
+        <v>13842.03061865115</v>
       </c>
       <c r="E81" t="n">
-        <v>336.4212323232325</v>
+        <v>-608.7233281363547</v>
       </c>
     </row>
     <row r="82">
@@ -1825,16 +1825,16 @@
         <v>1673.353535353535</v>
       </c>
       <c r="B82" t="n">
-        <v>483.654</v>
+        <v>7457090.351299997</v>
       </c>
       <c r="C82" t="n">
-        <v>0.08889999999999992</v>
+        <v>6271.500016686355</v>
       </c>
       <c r="D82" t="n">
-        <v>3433.008845627997</v>
+        <v>14140.20002367105</v>
       </c>
       <c r="E82" t="n">
-        <v>334.8928707070709</v>
+        <v>-613.1037675704973</v>
       </c>
     </row>
     <row r="83">
@@ -1842,16 +1842,16 @@
         <v>1690.545454545455</v>
       </c>
       <c r="B83" t="n">
-        <v>483.654</v>
+        <v>7699747.152799997</v>
       </c>
       <c r="C83" t="n">
-        <v>0.08889999999999992</v>
+        <v>6415.851362271853</v>
       </c>
       <c r="D83" t="n">
-        <v>3505.847117355372</v>
+        <v>14441.44327438016</v>
       </c>
       <c r="E83" t="n">
-        <v>333.3645090909092</v>
+        <v>-617.4925974646012</v>
       </c>
     </row>
     <row r="84">
@@ -1859,16 +1859,16 @@
         <v>1707.737373737374</v>
       </c>
       <c r="B84" t="n">
-        <v>483.654</v>
+        <v>7947490.614399996</v>
       </c>
       <c r="C84" t="n">
-        <v>0.08889999999999992</v>
+        <v>6561.753172273884</v>
       </c>
       <c r="D84" t="n">
-        <v>3579.4242942965</v>
+        <v>14745.76037077849</v>
       </c>
       <c r="E84" t="n">
-        <v>331.8361474747476</v>
+        <v>-621.8897637497445</v>
       </c>
     </row>
     <row r="85">
@@ -1876,16 +1876,16 @@
         <v>1724.929292929293</v>
       </c>
       <c r="B85" t="n">
-        <v>483.654</v>
+        <v>8200371.831299995</v>
       </c>
       <c r="C85" t="n">
-        <v>0.08889999999999992</v>
+        <v>6709.20450171855</v>
       </c>
       <c r="D85" t="n">
-        <v>3653.740376451382</v>
+        <v>15053.15131286603</v>
       </c>
       <c r="E85" t="n">
-        <v>330.307785858586</v>
+        <v>-626.2952134456928</v>
       </c>
     </row>
     <row r="86">
@@ -1893,16 +1893,16 @@
         <v>1742.121212121212</v>
       </c>
       <c r="B86" t="n">
-        <v>483.654</v>
+        <v>8473785.173399998</v>
       </c>
       <c r="C86" t="n">
-        <v>0.08889999999999992</v>
+        <v>6867.017342533542</v>
       </c>
       <c r="D86" t="n">
-        <v>3728.795363820018</v>
+        <v>15363.61610064279</v>
       </c>
       <c r="E86" t="n">
-        <v>328.7794242424244</v>
+        <v>-630.708894628345</v>
       </c>
     </row>
     <row r="87">
@@ -1910,16 +1910,16 @@
         <v>1759.313131313131</v>
       </c>
       <c r="B87" t="n">
-        <v>483.654</v>
+        <v>8737405.009799996</v>
       </c>
       <c r="C87" t="n">
-        <v>0.08889999999999992</v>
+        <v>7017.656000867034</v>
       </c>
       <c r="D87" t="n">
-        <v>3804.589256402407</v>
+        <v>15677.15473410876</v>
       </c>
       <c r="E87" t="n">
-        <v>327.2510626262628</v>
+        <v>-635.1307563984637</v>
       </c>
     </row>
     <row r="88">
@@ -1927,16 +1927,16 @@
         <v>1776.50505050505</v>
       </c>
       <c r="B88" t="n">
-        <v>483.654</v>
+        <v>9006318.892699994</v>
       </c>
       <c r="C88" t="n">
-        <v>0.08889999999999992</v>
+        <v>7169.841456319546</v>
       </c>
       <c r="D88" t="n">
-        <v>3881.122054198551</v>
+        <v>15993.76721326395</v>
       </c>
       <c r="E88" t="n">
-        <v>325.7227010101012</v>
+        <v>-639.5607488516299</v>
       </c>
     </row>
     <row r="89">
@@ -1944,16 +1944,16 @@
         <v>1793.69696969697</v>
       </c>
       <c r="B89" t="n">
-        <v>483.654</v>
+        <v>9280577.917299993</v>
       </c>
       <c r="C89" t="n">
-        <v>0.08889999999999992</v>
+        <v>7323.57287036181</v>
       </c>
       <c r="D89" t="n">
-        <v>3958.393757208447</v>
+        <v>16313.45353810835</v>
       </c>
       <c r="E89" t="n">
-        <v>324.1943393939396</v>
+        <v>-643.998823049358</v>
       </c>
     </row>
     <row r="90">
@@ -1961,16 +1961,16 @@
         <v>1810.888888888889</v>
       </c>
       <c r="B90" t="n">
-        <v>483.654</v>
+        <v>9560233.178799996</v>
       </c>
       <c r="C90" t="n">
-        <v>0.08889999999999992</v>
+        <v>7478.849428210406</v>
       </c>
       <c r="D90" t="n">
-        <v>4036.404365432098</v>
+        <v>16636.21370864197</v>
       </c>
       <c r="E90" t="n">
-        <v>322.6659777777779</v>
+        <v>-648.4449309913202</v>
       </c>
     </row>
     <row r="91">
@@ -1978,16 +1978,16 @@
         <v>1828.080808080808</v>
       </c>
       <c r="B91" t="n">
-        <v>483.654</v>
+        <v>9862277.245299993</v>
       </c>
       <c r="C91" t="n">
-        <v>0.08889999999999992</v>
+        <v>7644.943174775894</v>
       </c>
       <c r="D91" t="n">
-        <v>4115.153878869502</v>
+        <v>16962.0477248648</v>
       </c>
       <c r="E91" t="n">
-        <v>321.1376161616163</v>
+        <v>-652.899025588626</v>
       </c>
     </row>
     <row r="92">
@@ -1995,16 +1995,16 @@
         <v>1845.272727272727</v>
       </c>
       <c r="B92" t="n">
-        <v>483.654</v>
+        <v>10153203.29429999</v>
       </c>
       <c r="C92" t="n">
-        <v>0.08889999999999992</v>
+        <v>7803.398441889985</v>
       </c>
       <c r="D92" t="n">
-        <v>4194.64229752066</v>
+        <v>17290.95558677685</v>
       </c>
       <c r="E92" t="n">
-        <v>319.6092545454547</v>
+        <v>-657.3610606381052</v>
       </c>
     </row>
     <row r="93">
@@ -2012,16 +2012,16 @@
         <v>1862.464646464646</v>
       </c>
       <c r="B93" t="n">
-        <v>483.654</v>
+        <v>10449681.87139999</v>
       </c>
       <c r="C93" t="n">
-        <v>0.08889999999999992</v>
+        <v>7963.396498858237</v>
       </c>
       <c r="D93" t="n">
-        <v>4274.869621385573</v>
+        <v>17622.93729437812</v>
       </c>
       <c r="E93" t="n">
-        <v>318.0808929292931</v>
+        <v>-661.830990797551</v>
       </c>
     </row>
     <row r="94">
@@ -2029,16 +2029,16 @@
         <v>1879.656565656566</v>
       </c>
       <c r="B94" t="n">
-        <v>483.654</v>
+        <v>10751764.07179999</v>
       </c>
       <c r="C94" t="n">
-        <v>0.08889999999999992</v>
+        <v>8124.936618577276</v>
       </c>
       <c r="D94" t="n">
-        <v>4355.835850464238</v>
+        <v>17957.9928476686</v>
       </c>
       <c r="E94" t="n">
-        <v>316.5525313131315</v>
+        <v>-666.3087715618761</v>
       </c>
     </row>
     <row r="95">
@@ -2046,16 +2046,16 @@
         <v>1896.848484848485</v>
       </c>
       <c r="B95" t="n">
-        <v>483.654</v>
+        <v>11059500.99069999</v>
       </c>
       <c r="C95" t="n">
-        <v>0.08889999999999992</v>
+        <v>8288.018093595725</v>
       </c>
       <c r="D95" t="n">
-        <v>4437.540984756657</v>
+        <v>18296.1222466483</v>
       </c>
       <c r="E95" t="n">
-        <v>315.0241696969698</v>
+        <v>-670.794359240143</v>
       </c>
     </row>
     <row r="96">
@@ -2063,16 +2063,16 @@
         <v>1914.040404040404</v>
       </c>
       <c r="B96" t="n">
-        <v>483.654</v>
+        <v>11391560.31279999</v>
       </c>
       <c r="C96" t="n">
-        <v>0.08889999999999992</v>
+        <v>8462.371855642294</v>
       </c>
       <c r="D96" t="n">
-        <v>4519.98502426283</v>
+        <v>18637.32549131721</v>
       </c>
       <c r="E96" t="n">
-        <v>313.4958080808083</v>
+        <v>-675.2877109334237</v>
       </c>
     </row>
     <row r="97">
@@ -2080,16 +2080,16 @@
         <v>1931.232323232323</v>
       </c>
       <c r="B97" t="n">
-        <v>483.654</v>
+        <v>11711100.18719999</v>
       </c>
       <c r="C97" t="n">
-        <v>0.08889999999999992</v>
+        <v>8628.624561576979</v>
       </c>
       <c r="D97" t="n">
-        <v>4603.167968982756</v>
+        <v>18981.60258167534</v>
       </c>
       <c r="E97" t="n">
-        <v>311.9674464646466</v>
+        <v>-679.7887845134594</v>
       </c>
     </row>
     <row r="98">
@@ -2097,16 +2097,16 @@
         <v>1948.424242424242</v>
       </c>
       <c r="B98" t="n">
-        <v>483.654</v>
+        <v>12036451.07129999</v>
       </c>
       <c r="C98" t="n">
-        <v>0.08889999999999992</v>
+        <v>8796.416573652366</v>
       </c>
       <c r="D98" t="n">
-        <v>4687.089818916435</v>
+        <v>19328.95351772268</v>
       </c>
       <c r="E98" t="n">
-        <v>310.439084848485</v>
+        <v>-684.297538602076</v>
       </c>
     </row>
     <row r="99">
@@ -2114,16 +2114,16 @@
         <v>1965.616161616161</v>
       </c>
       <c r="B99" t="n">
-        <v>483.654</v>
+        <v>12367664.06029999</v>
       </c>
       <c r="C99" t="n">
-        <v>0.08889999999999992</v>
+        <v>8965.747257291594</v>
       </c>
       <c r="D99" t="n">
-        <v>4771.75057406387</v>
+        <v>19679.37829945923</v>
       </c>
       <c r="E99" t="n">
-        <v>308.9107232323234</v>
+        <v>-688.8139325513291</v>
       </c>
     </row>
     <row r="100">
@@ -2131,16 +2131,16 @@
         <v>1982.808080808081</v>
       </c>
       <c r="B100" t="n">
-        <v>483.654</v>
+        <v>12704790.24939999</v>
       </c>
       <c r="C100" t="n">
-        <v>0.08889999999999992</v>
+        <v>9136.615994321352</v>
       </c>
       <c r="D100" t="n">
-        <v>4857.150234425058</v>
+        <v>20032.876926885</v>
       </c>
       <c r="E100" t="n">
-        <v>307.3823616161618</v>
+        <v>-693.3379264243417</v>
       </c>
     </row>
     <row r="101">
@@ -2148,16 +2148,16 @@
         <v>2000</v>
       </c>
       <c r="B101" t="n">
-        <v>483.654</v>
+        <v>13068249.35829999</v>
       </c>
       <c r="C101" t="n">
-        <v>0.08889999999999992</v>
+        <v>9319.211589364839</v>
       </c>
       <c r="D101" t="n">
-        <v>4943.2888</v>
+        <v>20389.4494</v>
       </c>
       <c r="E101" t="n">
-        <v>305.8540000000002</v>
+        <v>-697.8694809768081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculation plot has been changed from using arange to to linspace for temperature ranges
</commit_message>
<xml_diff>
--- a/data_from_calculation.xlsx
+++ b/data_from_calculation.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,594 +414,1699 @@
         <v>298</v>
       </c>
       <c r="B2">
-        <v>0.0509</v>
+        <v>483.654</v>
       </c>
       <c r="C2">
-        <v>0.0509</v>
+        <v>0.08889999999999992</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>-1690.4422</v>
+        <v>457.1618</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>348</v>
+        <v>315.1919191919192</v>
       </c>
       <c r="B3">
-        <v>32240.76465</v>
+        <v>273.0988</v>
       </c>
       <c r="C3">
-        <v>97.51361758505345</v>
+        <v>-0.5925602990204895</v>
       </c>
       <c r="D3">
-        <v>1351.435</v>
+        <v>13.72585462707885</v>
       </c>
       <c r="E3">
-        <v>-1693.323090506074</v>
+        <v>455.6196076768169</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>398</v>
+        <v>332.3838383838384</v>
       </c>
       <c r="B4">
-        <v>137167.6034</v>
+        <v>-401.4169999999998</v>
       </c>
       <c r="C4">
-        <v>377.2769362948536</v>
+        <v>-2.67487193808215</v>
       </c>
       <c r="D4">
-        <v>2911.62</v>
+        <v>28.19061446791145</v>
       </c>
       <c r="E4">
-        <v>-1696.83228498559</v>
+        <v>454.0508066805136</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>448</v>
+        <v>349.5757575757576</v>
       </c>
       <c r="B5">
-        <v>325218.0671500001</v>
+        <v>-1565.440999999999</v>
       </c>
       <c r="C5">
-        <v>820.8225123021142</v>
+        <v>-6.09304709729517</v>
       </c>
       <c r="D5">
-        <v>4680.554999999999</v>
+        <v>43.39427952249769</v>
       </c>
       <c r="E5">
-        <v>-1700.916775094948</v>
+        <v>452.456854124249</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>498</v>
+        <v>366.7676767676768</v>
       </c>
       <c r="B6">
-        <v>606829.6559000002</v>
+        <v>-3244.5208</v>
       </c>
       <c r="C6">
-        <v>1415.537534076789</v>
+        <v>-10.79138949138432</v>
       </c>
       <c r="D6">
-        <v>6658.240000000001</v>
+        <v>59.33684979083769</v>
       </c>
       <c r="E6">
-        <v>-1705.535469616973</v>
+        <v>450.8390636183316</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>548</v>
+        <v>383.959595959596</v>
       </c>
       <c r="B7">
-        <v>992439.86965</v>
+        <v>-5464.204</v>
       </c>
       <c r="C7">
-        <v>2152.443233474342</v>
+        <v>-16.72180339677239</v>
       </c>
       <c r="D7">
-        <v>8844.674999999999</v>
+        <v>76.01832527293132</v>
       </c>
       <c r="E7">
-        <v>-1710.655575670596</v>
+        <v>449.1986254819113</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>598</v>
+        <v>401.1515151515151</v>
       </c>
       <c r="B8">
-        <v>1492486.2084</v>
+        <v>-8432.087799999999</v>
       </c>
       <c r="C8">
-        <v>3024.920341954929</v>
+        <v>-24.29759467275771</v>
       </c>
       <c r="D8">
-        <v>11239.86</v>
+        <v>93.43870596877866</v>
       </c>
       <c r="E8">
-        <v>-1716.250312297257</v>
+        <v>447.5366233280378</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>648</v>
+        <v>418.3434343434343</v>
       </c>
       <c r="B9">
-        <v>2117406.17215</v>
+        <v>-11845.222</v>
       </c>
       <c r="C9">
-        <v>4027.948542205007</v>
+        <v>-32.63874851530564</v>
       </c>
       <c r="D9">
-        <v>13843.795</v>
+        <v>111.5979918783797</v>
       </c>
       <c r="E9">
-        <v>-1722.297394253281</v>
+        <v>445.8540478008225</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>698</v>
+        <v>435.5353535353535</v>
       </c>
       <c r="B10">
-        <v>2877637.2609</v>
+        <v>-15877.1052</v>
       </c>
       <c r="C10">
-        <v>5157.629635827331</v>
+        <v>-42.09960129916492</v>
       </c>
       <c r="D10">
-        <v>16656.48</v>
+        <v>130.4961830017345</v>
       </c>
       <c r="E10">
-        <v>-1728.777986584576</v>
+        <v>444.1518080509884</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>748</v>
+        <v>452.7272727272727</v>
       </c>
       <c r="B11">
-        <v>3783616.97465</v>
+        <v>-20553.285</v>
       </c>
       <c r="C11">
-        <v>6410.876192804482</v>
+        <v>-52.65187548850506</v>
       </c>
       <c r="D11">
-        <v>19677.915</v>
+        <v>150.133279338843</v>
       </c>
       <c r="E11">
-        <v>-1735.675960277818</v>
+        <v>442.4307413969512</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>798</v>
+        <v>469.9191919191919</v>
       </c>
       <c r="B12">
-        <v>4845782.813400001</v>
+        <v>-25899.309</v>
       </c>
       <c r="C12">
-        <v>7785.201217978348</v>
+        <v>-64.27043017485137</v>
       </c>
       <c r="D12">
-        <v>22908.1</v>
+        <v>170.5092808897051</v>
       </c>
       <c r="E12">
-        <v>-1742.977347806657</v>
+        <v>440.6916215164968</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>848</v>
+        <v>487.1111111111111</v>
       </c>
       <c r="B13">
-        <v>6074572.277150001</v>
+        <v>-32318.30400000001</v>
       </c>
       <c r="C13">
-        <v>9278.571890129431</v>
+        <v>-77.70972560626115</v>
       </c>
       <c r="D13">
-        <v>26347.035</v>
+        <v>191.624187654321</v>
       </c>
       <c r="E13">
-        <v>-1750.669935651026</v>
+        <v>438.935165438245</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>898</v>
+        <v>504.3030303030303</v>
       </c>
       <c r="B14">
-        <v>7480422.865900001</v>
+        <v>-39123.863</v>
       </c>
       <c r="C14">
-        <v>10889.30529102039</v>
+        <v>-91.45543986379749</v>
       </c>
       <c r="D14">
-        <v>29994.72</v>
+        <v>213.4779996326905</v>
       </c>
       <c r="E14">
-        <v>-1758.742953240395</v>
+        <v>437.1620395449893</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>948</v>
+        <v>521.4949494949494</v>
       </c>
       <c r="B15">
-        <v>9073772.079649998</v>
+        <v>-46677.4118</v>
       </c>
       <c r="C15">
-        <v>12615.99244072141</v>
+        <v>-106.2057181850925</v>
       </c>
       <c r="D15">
-        <v>33851.15500000001</v>
+        <v>236.0707168248137</v>
       </c>
       <c r="E15">
-        <v>-1767.186831378563</v>
+        <v>435.3728647575559</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>998</v>
+        <v>538.6868686868686</v>
       </c>
       <c r="B16">
-        <v>10865057.4184</v>
+        <v>-55004.49800000001</v>
       </c>
       <c r="C16">
-        <v>14457.44189104965</v>
+        <v>-121.9442848260575</v>
       </c>
       <c r="D16">
-        <v>37916.34</v>
+        <v>259.4023392306906</v>
       </c>
       <c r="E16">
-        <v>-1775.993011767179</v>
+        <v>433.5682210344206</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>1048</v>
+        <v>555.8787878787879</v>
       </c>
       <c r="B17">
-        <v>12864716.38215</v>
+        <v>-64130.66920000001</v>
       </c>
       <c r="C17">
-        <v>16412.63712929963</v>
+        <v>-138.6563848187692</v>
       </c>
       <c r="D17">
-        <v>42190.275</v>
+        <v>283.4728668503214</v>
       </c>
       <c r="E17">
-        <v>-1785.153794790489</v>
+        <v>431.7486512963904</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>1098</v>
+        <v>573.070707070707</v>
       </c>
       <c r="B18">
-        <v>15083186.4709</v>
+        <v>-74693.041</v>
       </c>
       <c r="C18">
-        <v>18480.70392348648</v>
+        <v>-157.3977750408004</v>
       </c>
       <c r="D18">
-        <v>46672.96</v>
+        <v>308.2822996837057</v>
       </c>
       <c r="E18">
-        <v>-1794.662216410232</v>
+        <v>429.9146648653507</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>1148</v>
+        <v>590.2626262626262</v>
       </c>
       <c r="B19">
-        <v>17530905.18465002</v>
+        <v>-85544.83119999999</v>
       </c>
       <c r="C19">
-        <v>20660.88494854162</v>
+        <v>-176.0732674692618</v>
       </c>
       <c r="D19">
-        <v>51364.395</v>
+        <v>333.8306377308437</v>
       </c>
       <c r="E19">
-        <v>-1804.511947527019</v>
+        <v>428.0667404900357</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>1198</v>
+        <v>607.4545454545455</v>
       </c>
       <c r="B20">
-        <v>20218310.02340002</v>
+        <v>-97273.85199999998</v>
       </c>
       <c r="C20">
-        <v>22952.51982824354</v>
+        <v>-195.6848172023365</v>
       </c>
       <c r="D20">
-        <v>56264.58</v>
+        <v>360.1178809917356</v>
       </c>
       <c r="E20">
-        <v>-1814.697210905143</v>
+        <v>426.2053290190222</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>1248</v>
+        <v>624.6464646464647</v>
       </c>
       <c r="B21">
-        <v>23155838.48715001</v>
+        <v>-109905.651</v>
       </c>
       <c r="C21">
-        <v>25355.02926237836</v>
+        <v>-216.2222135434408</v>
       </c>
       <c r="D21">
-        <v>61373.51500000001</v>
+        <v>387.144029466381</v>
       </c>
       <c r="E21">
-        <v>-1825.212711988478</v>
+        <v>424.3308557709078</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>1298</v>
+        <v>641.8383838383838</v>
       </c>
       <c r="B22">
-        <v>26353928.07590001</v>
+        <v>-123465.7758</v>
       </c>
       <c r="C22">
-        <v>27867.90227502021</v>
+        <v>-237.6760699670341</v>
       </c>
       <c r="D22">
-        <v>66691.2</v>
+        <v>414.9090831547801</v>
       </c>
       <c r="E22">
-        <v>-1836.053580819785</v>
+        <v>422.4437226433806</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>1348</v>
+        <v>659.030303030303</v>
       </c>
       <c r="B23">
-        <v>29823016.28965002</v>
+        <v>-138863.79</v>
       </c>
       <c r="C23">
-        <v>30490.68587525671</v>
+        <v>-261.3812271004924</v>
       </c>
       <c r="D23">
-        <v>72217.63500000001</v>
+        <v>443.413042056933</v>
       </c>
       <c r="E23">
-        <v>-1847.215322921347</v>
+        <v>420.5443099961764</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>1398</v>
+        <v>676.2222222222222</v>
       </c>
       <c r="B24">
-        <v>33573540.62840002</v>
+        <v>-154415.6178</v>
       </c>
       <c r="C24">
-        <v>33222.97660258783</v>
+        <v>-284.6954151566463</v>
       </c>
       <c r="D24">
-        <v>77952.82000000001</v>
+        <v>472.6559061728394</v>
       </c>
       <c r="E24">
-        <v>-1858.693777472391</v>
+        <v>418.6329783374373</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>1448</v>
+        <v>693.4141414141413</v>
       </c>
       <c r="B25">
-        <v>37615938.59215002</v>
+        <v>-170973.917</v>
       </c>
       <c r="C25">
-        <v>36064.41355920507</v>
+        <v>-308.9016210447061</v>
       </c>
       <c r="D25">
-        <v>83896.755</v>
+        <v>502.6376755024996</v>
       </c>
       <c r="E25">
-        <v>-1870.485081476631</v>
+        <v>416.7100698384809</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>1498</v>
+        <v>710.6060606060605</v>
       </c>
       <c r="B26">
-        <v>41960647.68090004</v>
+        <v>-188564.2351999999</v>
       </c>
       <c r="C26">
-        <v>39014.67262599377</v>
+        <v>-333.9930234742147</v>
       </c>
       <c r="D26">
-        <v>90049.44</v>
+        <v>533.3583500459135</v>
       </c>
       <c r="E26">
-        <v>-1882.585638884345</v>
+        <v>414.7759096982641</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>1548</v>
+        <v>727.7979797979797</v>
       </c>
       <c r="B27">
-        <v>46618105.39465005</v>
+        <v>-207212.1199999999</v>
       </c>
       <c r="C27">
-        <v>42073.46162884836</v>
+        <v>-359.9632857689794</v>
       </c>
       <c r="D27">
-        <v>96410.875</v>
+        <v>564.8179298030811</v>
       </c>
       <c r="E27">
-        <v>-1894.992093841116</v>
+        <v>412.830807375736</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>1598</v>
+        <v>744.989898989899</v>
       </c>
       <c r="B28">
-        <v>51598749.23340004</v>
+        <v>-226943.1189999999</v>
       </c>
       <c r="C28">
-        <v>45240.51627388249</v>
+        <v>-386.8065110215546</v>
       </c>
       <c r="D28">
-        <v>102981.06</v>
+        <v>597.0164147740027</v>
       </c>
       <c r="E28">
-        <v>-1907.701307396039</v>
+        <v>410.8750577056919</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>1648</v>
+        <v>762.1818181818181</v>
       </c>
       <c r="B29">
-        <v>56913016.69715002</v>
+        <v>-249043.7139999999</v>
       </c>
       <c r="C29">
-        <v>48515.59670927815</v>
+        <v>-416.1741460762831</v>
       </c>
       <c r="D29">
-        <v>109759.995</v>
+        <v>629.9538049586777</v>
       </c>
       <c r="E29">
-        <v>-1920.710337127595</v>
+        <v>408.9089419115784</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>1698</v>
+        <v>779.3737373737373</v>
       </c>
       <c r="B30">
-        <v>62571345.28590005</v>
+        <v>-271085.0979999998</v>
       </c>
       <c r="C30">
-        <v>51898.48460130759</v>
+        <v>-444.7977440701821</v>
       </c>
       <c r="D30">
-        <v>116747.68</v>
+        <v>663.6301003571062</v>
       </c>
       <c r="E30">
-        <v>-1934.016419244126</v>
+        <v>406.9327285268777</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>1748</v>
+        <v>796.5656565656566</v>
       </c>
       <c r="B31">
-        <v>68584172.49965005</v>
+        <v>-294287.7417999998</v>
       </c>
       <c r="C31">
-        <v>55388.98063492848</v>
+        <v>-474.2786040236327</v>
       </c>
       <c r="D31">
-        <v>123944.115</v>
+        <v>698.0453009692889</v>
       </c>
       <c r="E31">
-        <v>-1947.616952794257</v>
+        <v>404.9466742351594</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>1798</v>
+        <v>813.7575757575758</v>
       </c>
       <c r="B32">
-        <v>74961935.83840002</v>
+        <v>-318677.1929999999</v>
       </c>
       <c r="C32">
-        <v>58986.90236705572</v>
+        <v>-504.6122486774791</v>
       </c>
       <c r="D32">
-        <v>131349.3</v>
+        <v>733.1994067952251</v>
       </c>
       <c r="E32">
-        <v>-1961.5094856852</v>
+        <v>402.9510246375812</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>1848</v>
+        <v>830.9494949494949</v>
       </c>
       <c r="B33">
-        <v>81715072.80215003</v>
+        <v>-344278.9991999999</v>
       </c>
       <c r="C33">
-        <v>62692.08237442818</v>
+        <v>-535.7944789379779</v>
       </c>
       <c r="D33">
-        <v>138963.235</v>
+        <v>769.0924178349148</v>
       </c>
       <c r="E33">
-        <v>-1975.691702257385</v>
+        <v>400.9460149555052</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
-        <v>1898</v>
+        <v>848.1414141414141</v>
       </c>
       <c r="B34">
-        <v>88854020.8909</v>
+        <v>-372736.6109999999</v>
       </c>
       <c r="C34">
-        <v>66504.36664885111</v>
+        <v>-569.7315083256718</v>
       </c>
       <c r="D34">
-        <v>146785.92</v>
+        <v>805.7243340883582</v>
       </c>
       <c r="E34">
-        <v>-1990.161412204691</v>
+        <v>398.9318706749466</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
-        <v>1948</v>
+        <v>865.3333333333333</v>
       </c>
       <c r="B35">
-        <v>96389217.60465004</v>
+        <v>-400914.8862000001</v>
       </c>
       <c r="C35">
-        <v>70423.61320119491</v>
+        <v>-602.6486704833223</v>
       </c>
       <c r="D35">
-        <v>154817.355</v>
+        <v>843.0951555555554</v>
       </c>
       <c r="E35">
-        <v>-2004.916540662909</v>
+        <v>396.9088081387495</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>1998</v>
+        <v>882.5252525252524</v>
       </c>
       <c r="B36">
-        <v>104331100.4434</v>
+        <v>-430383.6620000001</v>
       </c>
       <c r="C36">
-        <v>74449.69084238813</v>
+        <v>-636.403076180718</v>
       </c>
       <c r="D36">
-        <v>163057.54</v>
+        <v>881.2048822365064</v>
       </c>
       <c r="E36">
-        <v>-2019.955119316417</v>
+        <v>394.877035091689</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>899.7171717171717</v>
+      </c>
+      <c r="B37">
+        <v>-461168.486</v>
+      </c>
+      <c r="C37">
+        <v>-670.9914456977332</v>
+      </c>
+      <c r="D37">
+        <v>920.0535141312112</v>
+      </c>
+      <c r="E37">
+        <v>392.8367511830822</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>916.9090909090909</v>
+      </c>
+      <c r="B38">
+        <v>-493294.9057999999</v>
+      </c>
+      <c r="C38">
+        <v>-706.4106837528543</v>
+      </c>
+      <c r="D38">
+        <v>959.6410512396694</v>
+      </c>
+      <c r="E38">
+        <v>390.7881484309725</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>934.10101010101</v>
+      </c>
+      <c r="B39">
+        <v>-528801.8</v>
+      </c>
+      <c r="C39">
+        <v>-744.8157769674508</v>
+      </c>
+      <c r="D39">
+        <v>999.9674935618814</v>
+      </c>
+      <c r="E39">
+        <v>388.7314116514887</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>951.2929292929292</v>
+      </c>
+      <c r="B40">
+        <v>-563770.7727999999</v>
+      </c>
+      <c r="C40">
+        <v>-781.9365943185697</v>
+      </c>
+      <c r="D40">
+        <v>1041.032841097847</v>
+      </c>
+      <c r="E40">
+        <v>386.6667188565867</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>968.4848484848484</v>
+      </c>
+      <c r="B41">
+        <v>-600159.487</v>
+      </c>
+      <c r="C41">
+        <v>-819.8798215668254</v>
+      </c>
+      <c r="D41">
+        <v>1082.837093847566</v>
+      </c>
+      <c r="E41">
+        <v>384.5942416230302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>985.6767676767677</v>
+      </c>
+      <c r="B42">
+        <v>-637993.4902</v>
+      </c>
+      <c r="C42">
+        <v>-858.6429848164423</v>
+      </c>
+      <c r="D42">
+        <v>1125.38025181104</v>
+      </c>
+      <c r="E42">
+        <v>382.5141454351651</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>1002.868686868687</v>
+      </c>
+      <c r="B43">
+        <v>-677298.3299999997</v>
+      </c>
+      <c r="C43">
+        <v>-898.2237372424383</v>
+      </c>
+      <c r="D43">
+        <v>1168.662314988266</v>
+      </c>
+      <c r="E43">
+        <v>380.4265900037727</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>1020.060606060606</v>
+      </c>
+      <c r="B44">
+        <v>-720546.7721999997</v>
+      </c>
+      <c r="C44">
+        <v>-941.0214385617983</v>
+      </c>
+      <c r="D44">
+        <v>1212.683283379247</v>
+      </c>
+      <c r="E44">
+        <v>378.3317295630541</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>1037.252525252525</v>
+      </c>
+      <c r="B45">
+        <v>-762960.2489999995</v>
+      </c>
+      <c r="C45">
+        <v>-982.2785692102105</v>
+      </c>
+      <c r="D45">
+        <v>1257.443156983981</v>
+      </c>
+      <c r="E45">
+        <v>376.2297131475875</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>1054.444444444444</v>
+      </c>
+      <c r="B46">
+        <v>-806922.7079999994</v>
+      </c>
+      <c r="C46">
+        <v>-1024.346813489742</v>
+      </c>
+      <c r="D46">
+        <v>1302.941935802469</v>
+      </c>
+      <c r="E46">
+        <v>374.1206848509203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>1071.636363636364</v>
+      </c>
+      <c r="B47">
+        <v>-852459.6967999995</v>
+      </c>
+      <c r="C47">
+        <v>-1067.224259540498</v>
+      </c>
+      <c r="D47">
+        <v>1349.179619834711</v>
+      </c>
+      <c r="E47">
+        <v>372.0047840672918</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>1088.828282828283</v>
+      </c>
+      <c r="B48">
+        <v>-899596.7629999996</v>
+      </c>
+      <c r="C48">
+        <v>-1110.909085876164</v>
+      </c>
+      <c r="D48">
+        <v>1396.156209080706</v>
+      </c>
+      <c r="E48">
+        <v>369.8821457178423</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>1106.020202020202</v>
+      </c>
+      <c r="B49">
+        <v>-951279.0187999997</v>
+      </c>
+      <c r="C49">
+        <v>-1158.041695685809</v>
+      </c>
+      <c r="D49">
+        <v>1443.871703540455</v>
+      </c>
+      <c r="E49">
+        <v>367.7529004625305</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>1123.212121212121</v>
+      </c>
+      <c r="B50">
+        <v>-1001790.806</v>
+      </c>
+      <c r="C50">
+        <v>-1203.383395351197</v>
+      </c>
+      <c r="D50">
+        <v>1492.326103213957</v>
+      </c>
+      <c r="E50">
+        <v>365.6171748988741</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>1140.40404040404</v>
+      </c>
+      <c r="B51">
+        <v>-1053980.8162</v>
+      </c>
+      <c r="C51">
+        <v>-1249.52740826413</v>
+      </c>
+      <c r="D51">
+        <v>1541.519408101213</v>
+      </c>
+      <c r="E51">
+        <v>363.4750917485182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>1157.595959595959</v>
+      </c>
+      <c r="B52">
+        <v>-1107874.597</v>
+      </c>
+      <c r="C52">
+        <v>-1296.472226457337</v>
+      </c>
+      <c r="D52">
+        <v>1591.451618202223</v>
+      </c>
+      <c r="E52">
+        <v>361.3267700325529</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>1174.787878787879</v>
+      </c>
+      <c r="B53">
+        <v>-1163497.696</v>
+      </c>
+      <c r="C53">
+        <v>-1344.216407982337</v>
+      </c>
+      <c r="D53">
+        <v>1642.122733516988</v>
+      </c>
+      <c r="E53">
+        <v>359.1723252364128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>1191.979797979798</v>
+      </c>
+      <c r="B54">
+        <v>-1220875.6608</v>
+      </c>
+      <c r="C54">
+        <v>-1392.758573111074</v>
+      </c>
+      <c r="D54">
+        <v>1693.532754045505</v>
+      </c>
+      <c r="E54">
+        <v>357.0118694651233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>1209.171717171717</v>
+      </c>
+      <c r="B55">
+        <v>-1283569.935</v>
+      </c>
+      <c r="C55">
+        <v>-1445.024467032009</v>
+      </c>
+      <c r="D55">
+        <v>1745.681679787776</v>
+      </c>
+      <c r="E55">
+        <v>354.8455115895875</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>1226.363636363636</v>
+      </c>
+      <c r="B56">
+        <v>-1344641.3028</v>
+      </c>
+      <c r="C56">
+        <v>-1495.205441441941</v>
+      </c>
+      <c r="D56">
+        <v>1798.569510743801</v>
+      </c>
+      <c r="E56">
+        <v>352.6733573845535</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>1243.555555555555</v>
+      </c>
+      <c r="B57">
+        <v>-1407545.682</v>
+      </c>
+      <c r="C57">
+        <v>-1546.180529715835</v>
+      </c>
+      <c r="D57">
+        <v>1852.19624691358</v>
+      </c>
+      <c r="E57">
+        <v>350.4955096588426</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>1260.747474747475</v>
+      </c>
+      <c r="B58">
+        <v>-1472308.6202</v>
+      </c>
+      <c r="C58">
+        <v>-1597.948570911151</v>
+      </c>
+      <c r="D58">
+        <v>1906.561888297112</v>
+      </c>
+      <c r="E58">
+        <v>348.3120683783759</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>1277.939393939394</v>
+      </c>
+      <c r="B59">
+        <v>-1538955.665000001</v>
+      </c>
+      <c r="C59">
+        <v>-1650.508450782251</v>
+      </c>
+      <c r="D59">
+        <v>1961.666434894399</v>
+      </c>
+      <c r="E59">
+        <v>346.1231307824887</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>1295.131313131313</v>
+      </c>
+      <c r="B60">
+        <v>-1611605.127200001</v>
+      </c>
+      <c r="C60">
+        <v>-1707.021976588858</v>
+      </c>
+      <c r="D60">
+        <v>2017.509886705438</v>
+      </c>
+      <c r="E60">
+        <v>343.9287914939852</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>1312.323232323232</v>
+      </c>
+      <c r="B61">
+        <v>-1682211.659000001</v>
+      </c>
+      <c r="C61">
+        <v>-1761.208789836603</v>
+      </c>
+      <c r="D61">
+        <v>2074.092243730232</v>
+      </c>
+      <c r="E61">
+        <v>341.7291426233481</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>1329.515151515152</v>
+      </c>
+      <c r="B62">
+        <v>-1754780.443</v>
+      </c>
+      <c r="C62">
+        <v>-1816.184298341801</v>
+      </c>
+      <c r="D62">
+        <v>2131.413505968779</v>
+      </c>
+      <c r="E62">
+        <v>339.5242738674877</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>1346.707070707071</v>
+      </c>
+      <c r="B63">
+        <v>-1829337.0268</v>
+      </c>
+      <c r="C63">
+        <v>-1871.947553644845</v>
+      </c>
+      <c r="D63">
+        <v>2189.47367342108</v>
+      </c>
+      <c r="E63">
+        <v>337.3142726033819</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
+        <v>1363.89898989899</v>
+      </c>
+      <c r="B64">
+        <v>-1905906.958</v>
+      </c>
+      <c r="C64">
+        <v>-1928.497643012882</v>
+      </c>
+      <c r="D64">
+        <v>2248.272746087134</v>
+      </c>
+      <c r="E64">
+        <v>335.099223976934</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65">
+        <v>1381.090909090909</v>
+      </c>
+      <c r="B65">
+        <v>-1989203.8738</v>
+      </c>
+      <c r="C65">
+        <v>-1989.230854044499</v>
+      </c>
+      <c r="D65">
+        <v>2307.810723966942</v>
+      </c>
+      <c r="E65">
+        <v>332.8792109873494</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66">
+        <v>1398.282828282828</v>
+      </c>
+      <c r="B66">
+        <v>-2069999.376</v>
+      </c>
+      <c r="C66">
+        <v>-2047.398164672546</v>
+      </c>
+      <c r="D66">
+        <v>2368.087607060504</v>
+      </c>
+      <c r="E66">
+        <v>330.6543145673119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67">
+        <v>1415.474747474747</v>
+      </c>
+      <c r="B67">
+        <v>-2152886.371200001</v>
+      </c>
+      <c r="C67">
+        <v>-2106.349721280347</v>
+      </c>
+      <c r="D67">
+        <v>2429.103395367819</v>
+      </c>
+      <c r="E67">
+        <v>328.4246136592139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68">
+        <v>1432.666666666667</v>
+      </c>
+      <c r="B68">
+        <v>-2237890.407000001</v>
+      </c>
+      <c r="C68">
+        <v>-2166.084739044639</v>
+      </c>
+      <c r="D68">
+        <v>2490.858088888888</v>
+      </c>
+      <c r="E68">
+        <v>326.1901852876851</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69">
+        <v>1449.858585858586</v>
+      </c>
+      <c r="B69">
+        <v>-2325037.031000001</v>
+      </c>
+      <c r="C69">
+        <v>-2226.60246093929</v>
+      </c>
+      <c r="D69">
+        <v>2553.351687623711</v>
+      </c>
+      <c r="E69">
+        <v>323.951104628638</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70">
+        <v>1467.050505050505</v>
+      </c>
+      <c r="B70">
+        <v>-2419673.666000002</v>
+      </c>
+      <c r="C70">
+        <v>-2291.532357802159</v>
+      </c>
+      <c r="D70">
+        <v>2616.584191572288</v>
+      </c>
+      <c r="E70">
+        <v>321.7074450750384</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71">
+        <v>1484.242424242424</v>
+      </c>
+      <c r="B71">
+        <v>-2511311.945000002</v>
+      </c>
+      <c r="C71">
+        <v>-2353.659257175924</v>
+      </c>
+      <c r="D71">
+        <v>2680.555600734618</v>
+      </c>
+      <c r="E71">
+        <v>319.459278299593</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72">
+        <v>1501.434343434343</v>
+      </c>
+      <c r="B72">
+        <v>-2605170.957800002</v>
+      </c>
+      <c r="C72">
+        <v>-2416.56670444097</v>
+      </c>
+      <c r="D72">
+        <v>2745.265915110703</v>
+      </c>
+      <c r="E72">
+        <v>317.2066743145315</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>1518.626262626263</v>
+      </c>
+      <c r="B73">
+        <v>-2701276.252000001</v>
+      </c>
+      <c r="C73">
+        <v>-2480.254042831226</v>
+      </c>
+      <c r="D73">
+        <v>2810.715134700541</v>
+      </c>
+      <c r="E73">
+        <v>314.9497015286513</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>1535.818181818182</v>
+      </c>
+      <c r="B74">
+        <v>-2799653.375200001</v>
+      </c>
+      <c r="C74">
+        <v>-2544.720637531127</v>
+      </c>
+      <c r="D74">
+        <v>2876.903259504132</v>
+      </c>
+      <c r="E74">
+        <v>312.6884268017776</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>1553.010101010101</v>
+      </c>
+      <c r="B75">
+        <v>-2906321.995000001</v>
+      </c>
+      <c r="C75">
+        <v>-2613.82806542986</v>
+      </c>
+      <c r="D75">
+        <v>2943.830289521477</v>
+      </c>
+      <c r="E75">
+        <v>310.4229154967856</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>1570.20202020202</v>
+      </c>
+      <c r="B76">
+        <v>-3009456.857200001</v>
+      </c>
+      <c r="C76">
+        <v>-2679.897100815116</v>
+      </c>
+      <c r="D76">
+        <v>3011.496224752576</v>
+      </c>
+      <c r="E76">
+        <v>308.1532315293184</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>1587.393939393939</v>
+      </c>
+      <c r="B77">
+        <v>-3114941.694</v>
+      </c>
+      <c r="C77">
+        <v>-2746.743577135029</v>
+      </c>
+      <c r="D77">
+        <v>3079.901065197429</v>
+      </c>
+      <c r="E77">
+        <v>305.8794374153279</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>1604.585858585858</v>
+      </c>
+      <c r="B78">
+        <v>-3222802.053</v>
+      </c>
+      <c r="C78">
+        <v>-2814.366939269154</v>
+      </c>
+      <c r="D78">
+        <v>3149.044810856034</v>
+      </c>
+      <c r="E78">
+        <v>303.6015943165552</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>1621.777777777778</v>
+      </c>
+      <c r="B79">
+        <v>-3333063.4818</v>
+      </c>
+      <c r="C79">
+        <v>-2882.76664966045</v>
+      </c>
+      <c r="D79">
+        <v>3218.927461728394</v>
+      </c>
+      <c r="E79">
+        <v>301.319762084062</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>1638.969696969697</v>
+      </c>
+      <c r="B80">
+        <v>-3445751.528</v>
+      </c>
+      <c r="C80">
+        <v>-2951.942187582088</v>
+      </c>
+      <c r="D80">
+        <v>3289.549017814508</v>
+      </c>
+      <c r="E80">
+        <v>299.0339992999162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>1656.161616161616</v>
+      </c>
+      <c r="B81">
+        <v>-3567741.603800001</v>
+      </c>
+      <c r="C81">
+        <v>-3026.031939439104</v>
+      </c>
+      <c r="D81">
+        <v>3360.909479114375</v>
+      </c>
+      <c r="E81">
+        <v>296.7443633171281</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>1673.353535353535</v>
+      </c>
+      <c r="B82">
+        <v>-3685506.071</v>
+      </c>
+      <c r="C82">
+        <v>-3096.80319766918</v>
+      </c>
+      <c r="D82">
+        <v>3433.008845627997</v>
+      </c>
+      <c r="E82">
+        <v>294.4509102979279</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>1690.545454545455</v>
+      </c>
+      <c r="B83">
+        <v>-3805775.3012</v>
+      </c>
+      <c r="C83">
+        <v>-3168.348788004103</v>
+      </c>
+      <c r="D83">
+        <v>3505.847117355372</v>
+      </c>
+      <c r="E83">
+        <v>292.1536952504704</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>1707.737373737374</v>
+      </c>
+      <c r="B84">
+        <v>-3928574.842000001</v>
+      </c>
+      <c r="C84">
+        <v>-3240.66825124998</v>
+      </c>
+      <c r="D84">
+        <v>3579.4242942965</v>
+      </c>
+      <c r="E84">
+        <v>289.8527720640467</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>1724.929292929293</v>
+      </c>
+      <c r="B85">
+        <v>-4053930.241</v>
+      </c>
+      <c r="C85">
+        <v>-3313.761141868697</v>
+      </c>
+      <c r="D85">
+        <v>3653.740376451382</v>
+      </c>
+      <c r="E85">
+        <v>287.5481935428771</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>1742.121212121212</v>
+      </c>
+      <c r="B86">
+        <v>-4189473.676</v>
+      </c>
+      <c r="C86">
+        <v>-3391.996143007525</v>
+      </c>
+      <c r="D86">
+        <v>3728.795363820018</v>
+      </c>
+      <c r="E86">
+        <v>285.2400114385576</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>1759.313131313131</v>
+      </c>
+      <c r="B87">
+        <v>-4320171.58</v>
+      </c>
+      <c r="C87">
+        <v>-3466.680036510586</v>
+      </c>
+      <c r="D87">
+        <v>3804.589256402407</v>
+      </c>
+      <c r="E87">
+        <v>282.9282764812247</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>1776.50505050505</v>
+      </c>
+      <c r="B88">
+        <v>-4453503.487800001</v>
+      </c>
+      <c r="C88">
+        <v>-3542.136073860103</v>
+      </c>
+      <c r="D88">
+        <v>3881.122054198551</v>
+      </c>
+      <c r="E88">
+        <v>280.6130384095024</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>1793.69696969697</v>
+      </c>
+      <c r="B89">
+        <v>-4589494.947000002</v>
+      </c>
+      <c r="C89">
+        <v>-3618.363859704679</v>
+      </c>
+      <c r="D89">
+        <v>3958.393757208447</v>
+      </c>
+      <c r="E89">
+        <v>278.2943459992899</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>1810.888888888889</v>
+      </c>
+      <c r="B90">
+        <v>-4728171.5052</v>
+      </c>
+      <c r="C90">
+        <v>-3695.36300988866</v>
+      </c>
+      <c r="D90">
+        <v>4036.404365432098</v>
+      </c>
+      <c r="E90">
+        <v>275.9722470914451</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>1828.080808080808</v>
+      </c>
+      <c r="B91">
+        <v>-4877960.564999999</v>
+      </c>
+      <c r="C91">
+        <v>-3777.731867508444</v>
+      </c>
+      <c r="D91">
+        <v>4115.153878869502</v>
+      </c>
+      <c r="E91">
+        <v>273.6467886184174</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92">
+        <v>1845.272727272727</v>
+      </c>
+      <c r="B92">
+        <v>-5022245.712199999</v>
+      </c>
+      <c r="C92">
+        <v>-3856.317956580151</v>
+      </c>
+      <c r="D92">
+        <v>4194.64229752066</v>
+      </c>
+      <c r="E92">
+        <v>271.3180166298781</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93">
+        <v>1862.464646464646</v>
+      </c>
+      <c r="B93">
+        <v>-5169294.103999998</v>
+      </c>
+      <c r="C93">
+        <v>-3935.674300145354</v>
+      </c>
+      <c r="D93">
+        <v>4274.869621385573</v>
+      </c>
+      <c r="E93">
+        <v>268.9859763173953</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94">
+        <v>1879.656565656566</v>
+      </c>
+      <c r="B94">
+        <v>-5319131.287999998</v>
+      </c>
+      <c r="C94">
+        <v>-4015.800555387958</v>
+      </c>
+      <c r="D94">
+        <v>4355.835850464238</v>
+      </c>
+      <c r="E94">
+        <v>266.6507120381986</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95">
+        <v>1896.848484848485</v>
+      </c>
+      <c r="B95">
+        <v>-5471782.811799998</v>
+      </c>
+      <c r="C95">
+        <v>-4096.69638875742</v>
+      </c>
+      <c r="D95">
+        <v>4437.540984756657</v>
+      </c>
+      <c r="E95">
+        <v>264.3122673380735</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96">
+        <v>1914.040404040404</v>
+      </c>
+      <c r="B96">
+        <v>-5636509.761999999</v>
+      </c>
+      <c r="C96">
+        <v>-4183.189253473684</v>
+      </c>
+      <c r="D96">
+        <v>4519.98502426283</v>
+      </c>
+      <c r="E96">
+        <v>261.9706849734262</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97">
+        <v>1931.232323232323</v>
+      </c>
+      <c r="B97">
+        <v>-5795035.958799999</v>
+      </c>
+      <c r="C97">
+        <v>-4265.668499824355</v>
+      </c>
+      <c r="D97">
+        <v>4603.167968982756</v>
+      </c>
+      <c r="E97">
+        <v>259.6260069325546</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98">
+        <v>1948.424242424242</v>
+      </c>
+      <c r="B98">
+        <v>-5956454.640999998</v>
+      </c>
+      <c r="C98">
+        <v>-4348.916358160588</v>
+      </c>
+      <c r="D98">
+        <v>4687.089818916435</v>
+      </c>
+      <c r="E98">
+        <v>257.2782744561636</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99">
+        <v>1965.616161616161</v>
+      </c>
+      <c r="B99">
+        <v>-6120791.356199997</v>
+      </c>
+      <c r="C99">
+        <v>-4432.932529290862</v>
+      </c>
+      <c r="D99">
+        <v>4771.75057406387</v>
+      </c>
+      <c r="E99">
+        <v>254.927528057155</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>1982.808080808081</v>
+      </c>
+      <c r="B100">
+        <v>-6288071.651999996</v>
+      </c>
+      <c r="C100">
+        <v>-4517.716721757636</v>
+      </c>
+      <c r="D100">
+        <v>4857.150234425058</v>
+      </c>
+      <c r="E100">
+        <v>252.573807539725</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101">
+        <v>2000</v>
+      </c>
+      <c r="B101">
+        <v>-6468428.758199997</v>
+      </c>
+      <c r="C101">
+        <v>-4608.32502085771</v>
+      </c>
+      <c r="D101">
+        <v>4943.2888</v>
+      </c>
+      <c r="E101">
+        <v>250.2171520177995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current best version working
</commit_message>
<xml_diff>
--- a/data_from_calculation.xlsx
+++ b/data_from_calculation.xlsx
@@ -414,16 +414,16 @@
         <v>298</v>
       </c>
       <c r="B2">
-        <v>239.919</v>
+        <v>483.654</v>
       </c>
       <c r="C2">
-        <v>0.19</v>
+        <v>0.08889999999999992</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>183.299</v>
+        <v>457.1618</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -431,16 +431,16 @@
         <v>315.1919191919192</v>
       </c>
       <c r="B3">
-        <v>-320.8090000000001</v>
+        <v>246.5142</v>
       </c>
       <c r="C3">
-        <v>-1.624794565735266</v>
+        <v>-0.5925602990204895</v>
       </c>
       <c r="D3">
-        <v>14.19793778185897</v>
+        <v>13.72585462707885</v>
       </c>
       <c r="E3">
-        <v>180.0323066365554</v>
+        <v>455.6196076768169</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -448,16 +448,16 @@
         <v>332.3838383838384</v>
       </c>
       <c r="B4">
-        <v>-2116.3184</v>
+        <v>-456.0889999999998</v>
       </c>
       <c r="C4">
-        <v>-7.167760022038789</v>
+        <v>-2.67487193808215</v>
       </c>
       <c r="D4">
-        <v>29.16433698602184</v>
+        <v>28.19061446791145</v>
       </c>
       <c r="E4">
-        <v>176.7653172594256</v>
+        <v>454.0508066805136</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -465,16 +465,16 @@
         <v>349.5757575757576</v>
       </c>
       <c r="B5">
-        <v>-5213.426000000001</v>
+        <v>-1649.703199999999</v>
       </c>
       <c r="C5">
-        <v>-16.26248340670163</v>
+        <v>-6.09304709729517</v>
       </c>
       <c r="D5">
-        <v>44.89919761248851</v>
+        <v>43.39427952249769</v>
       </c>
       <c r="E5">
-        <v>173.4982552926284</v>
+        <v>452.456854124249</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -482,16 +482,16 @@
         <v>366.7676767676768</v>
       </c>
       <c r="B6">
-        <v>-9678.948600000003</v>
+        <v>-3359.876</v>
       </c>
       <c r="C6">
-        <v>-28.75777413222453</v>
+        <v>-10.79138949138432</v>
       </c>
       <c r="D6">
-        <v>61.40251966125907</v>
+        <v>59.33684979083769</v>
       </c>
       <c r="E6">
-        <v>170.2313221564112</v>
+        <v>450.8390636183316</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -499,16 +499,16 @@
         <v>383.959595959596</v>
       </c>
       <c r="B7">
-        <v>-15579.70300000001</v>
+        <v>-5612.155000000001</v>
       </c>
       <c r="C7">
-        <v>-44.5230737481128</v>
+        <v>-16.72180339677239</v>
       </c>
       <c r="D7">
-        <v>78.67430313233342</v>
+        <v>76.01832527293132</v>
       </c>
       <c r="E7">
-        <v>166.9647003663768</v>
+        <v>449.1986254819113</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -516,16 +516,16 @@
         <v>401.1515151515151</v>
       </c>
       <c r="B8">
-        <v>-23466.16960000001</v>
+        <v>-8616.189999999999</v>
       </c>
       <c r="C8">
-        <v>-64.65402364310089</v>
+        <v>-24.29759467275771</v>
       </c>
       <c r="D8">
-        <v>96.71454802571162</v>
+        <v>93.43870596877866</v>
       </c>
       <c r="E8">
-        <v>163.6985560765262</v>
+        <v>447.5366233280378</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -533,16 +533,16 @@
         <v>418.3434343434343</v>
       </c>
       <c r="B9">
-        <v>-32532.20500000002</v>
+        <v>-12065.014</v>
       </c>
       <c r="C9">
-        <v>-86.80999217003885</v>
+        <v>-32.63874851530564</v>
       </c>
       <c r="D9">
-        <v>115.5232543413937</v>
+        <v>111.5979918783797</v>
       </c>
       <c r="E9">
-        <v>160.4330411856232</v>
+        <v>445.8540478008225</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -550,16 +550,16 @@
         <v>435.5353535353535</v>
       </c>
       <c r="B10">
-        <v>-43237.85300000003</v>
+        <v>-16134.0898</v>
       </c>
       <c r="C10">
-        <v>-111.9309281507138</v>
+        <v>-42.09960129916492</v>
       </c>
       <c r="D10">
-        <v>135.1004220793797</v>
+        <v>130.4961830017345</v>
       </c>
       <c r="E10">
-        <v>157.1682950967786</v>
+        <v>444.1518080509884</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -567,16 +567,16 @@
         <v>452.7272727272727</v>
       </c>
       <c r="B11">
-        <v>-55649.93040000004</v>
+        <v>-20848.965</v>
       </c>
       <c r="C11">
-        <v>-139.9400706802625</v>
+        <v>-52.65187548850506</v>
       </c>
       <c r="D11">
-        <v>155.4460512396695</v>
+        <v>150.133279338843</v>
       </c>
       <c r="E11">
-        <v>153.9044461988162</v>
+        <v>442.4307413969512</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -584,16 +584,16 @@
         <v>469.9191919191919</v>
       </c>
       <c r="B12">
-        <v>-69835.25400000006</v>
+        <v>-26235.1872</v>
       </c>
       <c r="C12">
-        <v>-170.7691733989183</v>
+        <v>-64.27043017485137</v>
       </c>
       <c r="D12">
-        <v>176.560141822263</v>
+        <v>170.5092808897051</v>
       </c>
       <c r="E12">
-        <v>150.6416131223298</v>
+        <v>440.6916215164968</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -601,16 +601,16 @@
         <v>487.1111111111111</v>
       </c>
       <c r="B13">
-        <v>-86862.04140000005</v>
+        <v>-32698.38300000001</v>
       </c>
       <c r="C13">
-        <v>-206.4177854601755</v>
+        <v>-77.70972560626115</v>
       </c>
       <c r="D13">
-        <v>198.4426938271604</v>
+        <v>191.624187654321</v>
       </c>
       <c r="E13">
-        <v>147.3799058117078</v>
+        <v>438.935165438245</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -618,16 +618,16 @@
         <v>504.3030303030303</v>
       </c>
       <c r="B14">
-        <v>-104908.558</v>
+        <v>-39547.2342</v>
       </c>
       <c r="C14">
-        <v>-242.8677628042772</v>
+        <v>-91.45543986379749</v>
       </c>
       <c r="D14">
-        <v>221.0937072543617</v>
+        <v>213.4779996326905</v>
       </c>
       <c r="E14">
-        <v>144.1194264456452</v>
+        <v>437.1620395449893</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -635,16 +635,16 @@
         <v>521.4949494949494</v>
       </c>
       <c r="B15">
-        <v>-124932.7016000001</v>
+        <v>-47145.578</v>
       </c>
       <c r="C15">
-        <v>-281.9701677317668</v>
+        <v>-106.2057181850925</v>
       </c>
       <c r="D15">
-        <v>244.5131821038669</v>
+        <v>236.0707168248137</v>
       </c>
       <c r="E15">
-        <v>140.860270232002</v>
+        <v>435.3728647575559</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -652,16 +652,16 @@
         <v>538.6868686868686</v>
       </c>
       <c r="B16">
-        <v>-147001.2890000001</v>
+        <v>-55518.96200000001</v>
       </c>
       <c r="C16">
-        <v>-323.6808188524743</v>
+        <v>-121.9442848260575</v>
       </c>
       <c r="D16">
-        <v>268.7011183756758</v>
+        <v>259.4023392306906</v>
       </c>
       <c r="E16">
-        <v>137.6025260977444</v>
+        <v>433.5682210344206</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -669,16 +669,16 @@
         <v>555.8787878787879</v>
       </c>
       <c r="B17">
-        <v>-171181.1370000001</v>
+        <v>-64692.93380000001</v>
       </c>
       <c r="C17">
-        <v>-367.9596630056222</v>
+        <v>-138.6563848187692</v>
       </c>
       <c r="D17">
-        <v>293.6575160697888</v>
+        <v>283.4728668503214</v>
       </c>
       <c r="E17">
-        <v>134.3462772907296</v>
+        <v>431.7486512963904</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -686,16 +686,16 @@
         <v>573.070707070707</v>
       </c>
       <c r="B18">
-        <v>-199158.7860000001</v>
+        <v>-75307.556</v>
       </c>
       <c r="C18">
-        <v>-417.6019610600028</v>
+        <v>-157.3977750408004</v>
       </c>
       <c r="D18">
-        <v>319.3823751862055</v>
+        <v>308.2822996837057</v>
       </c>
       <c r="E18">
-        <v>131.0916019069801</v>
+        <v>429.9146648653507</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -703,16 +703,16 @@
         <v>590.2626262626262</v>
       </c>
       <c r="B19">
-        <v>-227895.7390000001</v>
+        <v>-86210.24079999999</v>
       </c>
       <c r="C19">
-        <v>-467.0571250662638</v>
+        <v>-176.0732674692618</v>
       </c>
       <c r="D19">
-        <v>345.8756957249259</v>
+        <v>333.8306377308437</v>
       </c>
       <c r="E19">
-        <v>127.8385733546349</v>
+        <v>428.0667404900357</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -720,16 +720,16 @@
         <v>607.4545454545455</v>
       </c>
       <c r="B20">
-        <v>-258948.3334000001</v>
+        <v>-97991.65899999999</v>
       </c>
       <c r="C20">
-        <v>-518.9787513422179</v>
+        <v>-195.6848172023365</v>
       </c>
       <c r="D20">
-        <v>373.1374776859505</v>
+        <v>360.1178809917356</v>
       </c>
       <c r="E20">
-        <v>124.5872607638093</v>
+        <v>426.2053290190222</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -737,16 +737,16 @@
         <v>624.6464646464647</v>
       </c>
       <c r="B21">
-        <v>-292383.3860000002</v>
+        <v>-110677.3582</v>
       </c>
       <c r="C21">
-        <v>-573.339122398132</v>
+        <v>-216.2222135434408</v>
       </c>
       <c r="D21">
-        <v>401.1677210692786</v>
+        <v>387.144029466381</v>
       </c>
       <c r="E21">
-        <v>121.3377293500215</v>
+        <v>424.3308557709078</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -754,16 +754,16 @@
         <v>641.8383838383838</v>
       </c>
       <c r="B22">
-        <v>-328267.7136000001</v>
+        <v>-124292.886</v>
       </c>
       <c r="C22">
-        <v>-630.1127580012746</v>
+        <v>-237.6760699670341</v>
       </c>
       <c r="D22">
-        <v>429.9664258749107</v>
+        <v>414.9090831547801</v>
       </c>
       <c r="E22">
-        <v>118.0900407375837</v>
+        <v>422.4437226433806</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -771,16 +771,16 @@
         <v>659.030303030303</v>
       </c>
       <c r="B23">
-        <v>-369006.7650000001</v>
+        <v>-139751.2002</v>
       </c>
       <c r="C23">
-        <v>-692.8303326688713</v>
+        <v>-261.3812271004924</v>
       </c>
       <c r="D23">
-        <v>459.5335921028466</v>
+        <v>443.413042056933</v>
       </c>
       <c r="E23">
-        <v>114.8442532483222</v>
+        <v>420.5443099961764</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -788,16 +788,16 @@
         <v>676.2222222222222</v>
       </c>
       <c r="B24">
-        <v>-410144.1096000001</v>
+        <v>-155361.525</v>
       </c>
       <c r="C24">
-        <v>-754.5005239845701</v>
+        <v>-284.6954151566463</v>
       </c>
       <c r="D24">
-        <v>489.8692197530863</v>
+        <v>472.6559061728394</v>
       </c>
       <c r="E24">
-        <v>111.6004221601519</v>
+        <v>418.6329783374373</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -805,16 +805,16 @@
         <v>693.4141414141413</v>
       </c>
       <c r="B25">
-        <v>-453935.1099999999</v>
+        <v>-171979.824</v>
       </c>
       <c r="C25">
-        <v>-818.5176300324745</v>
+        <v>-308.9016210447061</v>
       </c>
       <c r="D25">
-        <v>520.9733088256298</v>
+        <v>502.6376755024996</v>
       </c>
       <c r="E25">
-        <v>108.3585999393416</v>
+        <v>416.7100698384809</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -822,16 +822,16 @@
         <v>710.6060606060605</v>
       </c>
       <c r="B26">
-        <v>-500446.583</v>
+        <v>-189631.6448</v>
       </c>
       <c r="C26">
-        <v>-884.8631340496338</v>
+        <v>-333.9930234742147</v>
       </c>
       <c r="D26">
-        <v>552.8458593204773</v>
+        <v>533.3583500459135</v>
       </c>
       <c r="E26">
-        <v>105.1188364497314</v>
+        <v>414.7759096982641</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -839,16 +839,16 @@
         <v>727.7979797979797</v>
       </c>
       <c r="B27">
-        <v>-549745.3453999998</v>
+        <v>-208342.5349999999</v>
       </c>
       <c r="C27">
-        <v>-953.5198347848042</v>
+        <v>-359.9632857689794</v>
       </c>
       <c r="D27">
-        <v>585.4868712376286</v>
+        <v>564.8179298030811</v>
       </c>
       <c r="E27">
-        <v>101.8811791416934</v>
+        <v>412.830807375736</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -856,16 +856,16 @@
         <v>744.989898989899</v>
       </c>
       <c r="B28">
-        <v>-601898.2139999996</v>
+        <v>-228138.0421999999</v>
       </c>
       <c r="C28">
-        <v>-1024.471724762861</v>
+        <v>-386.8065110215546</v>
       </c>
       <c r="D28">
-        <v>618.8963445770839</v>
+        <v>597.0164147740027</v>
       </c>
       <c r="E28">
-        <v>98.64567322322956</v>
+        <v>410.8750577056919</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -873,16 +873,16 @@
         <v>762.1818181818181</v>
       </c>
       <c r="B29">
-        <v>-660304.0313999995</v>
+        <v>-250308.5779999999</v>
       </c>
       <c r="C29">
-        <v>-1102.082365624367</v>
+        <v>-416.1741460762831</v>
       </c>
       <c r="D29">
-        <v>653.0742793388429</v>
+        <v>629.9538049586777</v>
       </c>
       <c r="E29">
-        <v>95.41236181526844</v>
+        <v>408.9089419115784</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -890,16 +890,16 @@
         <v>779.3737373737373</v>
       </c>
       <c r="B30">
-        <v>-718543.3929999995</v>
+        <v>-272417.5641999998</v>
       </c>
       <c r="C30">
-        <v>-1177.713758567527</v>
+        <v>-444.7977440701821</v>
       </c>
       <c r="D30">
-        <v>688.0206755229057</v>
+        <v>663.6301003571062</v>
       </c>
       <c r="E30">
-        <v>92.18128609294394</v>
+        <v>406.9327285268777</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -907,16 +907,16 @@
         <v>796.5656565656566</v>
       </c>
       <c r="B31">
-        <v>-779841.2415999993</v>
+        <v>-295689.3129999998</v>
       </c>
       <c r="C31">
-        <v>-1255.597719542132</v>
+        <v>-474.2786040236327</v>
       </c>
       <c r="D31">
-        <v>723.7355331292725</v>
+        <v>698.0453009692889</v>
       </c>
       <c r="E31">
-        <v>88.95248541440334</v>
+        <v>404.9466742351594</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -924,16 +924,16 @@
         <v>813.7575757575758</v>
       </c>
       <c r="B32">
-        <v>-844264.3939999993</v>
+        <v>-320149.3719999999</v>
       </c>
       <c r="C32">
-        <v>-1335.722094785348</v>
+        <v>-504.6122486774791</v>
       </c>
       <c r="D32">
-        <v>760.218852157943</v>
+        <v>733.1994067952251</v>
       </c>
       <c r="E32">
-        <v>85.72599743849091</v>
+        <v>402.9510246375812</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -941,16 +941,16 @@
         <v>830.9494949494949</v>
       </c>
       <c r="B33">
-        <v>-911879.6669999992</v>
+        <v>-345823.2887999999</v>
       </c>
       <c r="C33">
-        <v>-1418.075485629435</v>
+        <v>-535.7944789379779</v>
       </c>
       <c r="D33">
-        <v>797.4706326089174</v>
+        <v>769.0924178349148</v>
       </c>
       <c r="E33">
-        <v>82.50185823248214</v>
+        <v>400.9460149555052</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -958,16 +958,16 @@
         <v>848.1414141414141</v>
       </c>
       <c r="B34">
-        <v>-987025.8659999993</v>
+        <v>-374358.8909999999</v>
       </c>
       <c r="C34">
-        <v>-1507.69085734807</v>
+        <v>-569.7315083256718</v>
       </c>
       <c r="D34">
-        <v>835.4908744821955</v>
+        <v>805.7243340883582</v>
       </c>
       <c r="E34">
-        <v>79.28010237089933</v>
+        <v>398.9318706749466</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -975,16 +975,16 @@
         <v>865.3333333333333</v>
       </c>
       <c r="B35">
-        <v>-1061423.543999999</v>
+        <v>-402612.3708000001</v>
       </c>
       <c r="C35">
-        <v>-1594.60039952092</v>
+        <v>-602.6486704833223</v>
       </c>
       <c r="D35">
-        <v>874.2795777777776</v>
+        <v>843.0951555555554</v>
       </c>
       <c r="E35">
-        <v>76.06076302631195</v>
+        <v>396.9088081387495</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -992,16 +992,16 @@
         <v>882.5252525252524</v>
       </c>
       <c r="B36">
-        <v>-1139217.723399999</v>
+        <v>-432157.8540000001</v>
       </c>
       <c r="C36">
-        <v>-1683.708168638797</v>
+        <v>-636.403076180718</v>
       </c>
       <c r="D36">
-        <v>913.8367424956634</v>
+        <v>881.2048822365064</v>
       </c>
       <c r="E36">
-        <v>72.84387205291881</v>
+        <v>394.877035091689</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1009,16 +1009,16 @@
         <v>899.7171717171717</v>
       </c>
       <c r="B37">
-        <v>-1220475.220999999</v>
+        <v>-463020.8882</v>
       </c>
       <c r="C37">
-        <v>-1775.005261723519</v>
+        <v>-670.9914456977332</v>
       </c>
       <c r="D37">
-        <v>954.1623686358535</v>
+        <v>920.0535141312112</v>
       </c>
       <c r="E37">
-        <v>69.6294600636152</v>
+        <v>392.8367511830822</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1026,16 +1026,16 @@
         <v>916.9090909090909</v>
       </c>
       <c r="B38">
-        <v>-1305262.8536</v>
+        <v>-495227.0209999999</v>
       </c>
       <c r="C38">
-        <v>-1868.483276465522</v>
+        <v>-706.4106837528543</v>
       </c>
       <c r="D38">
-        <v>995.256456198347</v>
+        <v>959.6410512396694</v>
       </c>
       <c r="E38">
-        <v>66.41755650116781</v>
+        <v>390.7881484309725</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1043,16 +1043,16 @@
         <v>934.10101010101</v>
       </c>
       <c r="B39">
-        <v>-1398959.975</v>
+        <v>-530819.9552000001</v>
       </c>
       <c r="C39">
-        <v>-1969.828311886132</v>
+        <v>-744.8157769674508</v>
       </c>
       <c r="D39">
-        <v>1037.119005183145</v>
+        <v>999.9674935618814</v>
       </c>
       <c r="E39">
-        <v>63.20818970404971</v>
+        <v>388.7314116514887</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1060,16 +1060,16 @@
         <v>951.2929292929292</v>
       </c>
       <c r="B40">
-        <v>-1491225.9246</v>
+        <v>-565871.7349999999</v>
       </c>
       <c r="C40">
-        <v>-2067.771940511926</v>
+        <v>-781.9365943185697</v>
       </c>
       <c r="D40">
-        <v>1079.750015590246</v>
+        <v>1041.032841097847</v>
       </c>
       <c r="E40">
-        <v>60.00138696742748</v>
+        <v>386.6667188565867</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1077,16 +1077,16 @@
         <v>968.4848484848484</v>
       </c>
       <c r="B41">
-        <v>-1587226.39</v>
+        <v>-602344.759</v>
       </c>
       <c r="C41">
-        <v>-2167.873529355272</v>
+        <v>-819.8798215668254</v>
       </c>
       <c r="D41">
-        <v>1123.149487419651</v>
+        <v>1082.837093847566</v>
       </c>
       <c r="E41">
-        <v>56.7971745997382</v>
+        <v>384.5942416230302</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1094,16 +1094,16 @@
         <v>985.6767676767677</v>
       </c>
       <c r="B42">
-        <v>-1687028.188</v>
+        <v>-640264.5747999999</v>
       </c>
       <c r="C42">
-        <v>-2270.126362891894</v>
+        <v>-858.6429848164423</v>
       </c>
       <c r="D42">
-        <v>1167.31742067136</v>
+        <v>1125.38025181104</v>
       </c>
       <c r="E42">
-        <v>53.59557797524821</v>
+        <v>382.5141454351651</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1111,16 +1111,16 @@
         <v>1002.868686868687</v>
       </c>
       <c r="B43">
-        <v>-1790698.1354</v>
+        <v>-679656.7299999997</v>
       </c>
       <c r="C43">
-        <v>-2374.524070538077</v>
+        <v>-898.2237372424383</v>
       </c>
       <c r="D43">
-        <v>1212.253815345373</v>
+        <v>1168.662314988266</v>
       </c>
       <c r="E43">
-        <v>50.39662158294406</v>
+        <v>380.4265900037727</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1128,16 +1128,16 @@
         <v>1020.060606060606</v>
       </c>
       <c r="B44">
-        <v>-1904756.72</v>
+        <v>-722999.2617999996</v>
       </c>
       <c r="C44">
-        <v>-2487.393941009992</v>
+        <v>-941.0214385617983</v>
       </c>
       <c r="D44">
-        <v>1257.958671441689</v>
+        <v>1212.683283379247</v>
       </c>
       <c r="E44">
-        <v>47.20032907206986</v>
+        <v>378.3317295630541</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1145,16 +1145,16 @@
         <v>1037.252525252525</v>
       </c>
       <c r="B45">
-        <v>-2016600.8964</v>
+        <v>-765503.1479999995</v>
       </c>
       <c r="C45">
-        <v>-2596.188852858756</v>
+        <v>-982.2785692102105</v>
       </c>
       <c r="D45">
-        <v>1304.43198896031</v>
+        <v>1257.443156983981</v>
       </c>
       <c r="E45">
-        <v>44.00672329459428</v>
+        <v>376.2297131475875</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1162,16 +1162,16 @@
         <v>1054.444444444444</v>
       </c>
       <c r="B46">
-        <v>-2132517.602999999</v>
+        <v>-809557.5191999994</v>
       </c>
       <c r="C46">
-        <v>-2707.111060598225</v>
+        <v>-1024.346813489742</v>
       </c>
       <c r="D46">
-        <v>1351.673767901234</v>
+        <v>1302.941935802469</v>
       </c>
       <c r="E46">
-        <v>40.81582634486124</v>
+        <v>374.1206848509203</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1179,16 +1179,16 @@
         <v>1071.636363636364</v>
       </c>
       <c r="B47">
-        <v>-2252573.656599999</v>
+        <v>-855187.9229999995</v>
       </c>
       <c r="C47">
-        <v>-2820.15537438101</v>
+        <v>-1067.224259540498</v>
       </c>
       <c r="D47">
-        <v>1399.684008264462</v>
+        <v>1349.179619834711</v>
       </c>
       <c r="E47">
-        <v>37.62765959665415</v>
+        <v>372.0047840672918</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1196,16 +1196,16 @@
         <v>1088.828282828283</v>
       </c>
       <c r="B48">
-        <v>-2376835.874</v>
+        <v>-902419.9069999995</v>
       </c>
       <c r="C48">
-        <v>-2935.316849683708</v>
+        <v>-1110.909085876164</v>
       </c>
       <c r="D48">
-        <v>1448.462710049994</v>
+        <v>1396.156209080706</v>
       </c>
       <c r="E48">
-        <v>34.44224373788113</v>
+        <v>369.8821457178423</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1213,16 +1213,16 @@
         <v>1106.020202020202</v>
       </c>
       <c r="B49">
-        <v>-2513066.4626</v>
+        <v>-954204.3019999997</v>
       </c>
       <c r="C49">
-        <v>-3059.554926473641</v>
+        <v>-1158.041695685809</v>
       </c>
       <c r="D49">
-        <v>1498.00987325783</v>
+        <v>1443.871703540455</v>
       </c>
       <c r="E49">
-        <v>31.25959880306921</v>
+        <v>367.7529004625305</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1230,16 +1230,16 @@
         <v>1123.212121212121</v>
       </c>
       <c r="B50">
-        <v>-2646198.820999999</v>
+        <v>-1004814.101</v>
       </c>
       <c r="C50">
-        <v>-3179.0606588897</v>
+        <v>-1203.383395351197</v>
       </c>
       <c r="D50">
-        <v>1548.32549788797</v>
+        <v>1492.326103213957</v>
       </c>
       <c r="E50">
-        <v>28.07974420383777</v>
+        <v>365.6171748988741</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1247,16 +1247,16 @@
         <v>1140.40404040404</v>
       </c>
       <c r="B51">
-        <v>-2783741.723999999</v>
+        <v>-1057103.6258</v>
       </c>
       <c r="C51">
-        <v>-3300.669798077897</v>
+        <v>-1249.52740826413</v>
       </c>
       <c r="D51">
-        <v>1599.409583940413</v>
+        <v>1541.519408101213</v>
       </c>
       <c r="E51">
-        <v>24.90269875750571</v>
+        <v>363.4750917485182</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1264,16 +1264,16 @@
         <v>1157.595959595959</v>
       </c>
       <c r="B52">
-        <v>-2925761.988399999</v>
+        <v>-1111098.424</v>
       </c>
       <c r="C52">
-        <v>-3424.378250579272</v>
+        <v>-1296.472226457337</v>
       </c>
       <c r="D52">
-        <v>1651.262131415161</v>
+        <v>1591.451618202223</v>
       </c>
       <c r="E52">
-        <v>21.72848071397352</v>
+        <v>361.3267700325529</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1281,16 +1281,16 @@
         <v>1174.787878787879</v>
       </c>
       <c r="B53">
-        <v>-3072326.430999998</v>
+        <v>-1166824.0432</v>
       </c>
       <c r="C53">
-        <v>-3550.182102146466</v>
+        <v>-1344.216407982337</v>
       </c>
       <c r="D53">
-        <v>1703.883140312213</v>
+        <v>1642.122733516988</v>
       </c>
       <c r="E53">
-        <v>18.5571077810078</v>
+        <v>359.1723252364128</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1298,16 +1298,16 @@
         <v>1191.979797979798</v>
       </c>
       <c r="B54">
-        <v>-3223501.868599998</v>
+        <v>-1224306.031</v>
       </c>
       <c r="C54">
-        <v>-3678.077607432825</v>
+        <v>-1392.758573111074</v>
       </c>
       <c r="D54">
-        <v>1757.272610631568</v>
+        <v>1693.532754045505</v>
       </c>
       <c r="E54">
-        <v>15.38859714804587</v>
+        <v>357.0118694651233</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1315,16 +1315,16 @@
         <v>1209.171717171717</v>
       </c>
       <c r="B55">
-        <v>-3388670.059999998</v>
+        <v>-1287112.0852</v>
       </c>
       <c r="C55">
-        <v>-3815.772225114548</v>
+        <v>-1445.024467032009</v>
       </c>
       <c r="D55">
-        <v>1811.430542373227</v>
+        <v>1745.681679787776</v>
       </c>
       <c r="E55">
-        <v>12.22296550862616</v>
+        <v>354.8455115895875</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1332,16 +1332,16 @@
         <v>1226.363636363636</v>
       </c>
       <c r="B56">
-        <v>-3549549.114599998</v>
+        <v>-1348290.57</v>
       </c>
       <c r="C56">
-        <v>-3947.962951674697</v>
+        <v>-1495.205441441941</v>
       </c>
       <c r="D56">
-        <v>1866.35693553719</v>
+        <v>1798.569510743801</v>
       </c>
       <c r="E56">
-        <v>9.060229081543351</v>
+        <v>352.6733573845535</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1349,16 +1349,16 @@
         <v>1243.555555555555</v>
       </c>
       <c r="B57">
-        <v>-3715243.544999997</v>
+        <v>-1411303.569</v>
       </c>
       <c r="C57">
-        <v>-4082.234827335493</v>
+        <v>-1546.180529715835</v>
       </c>
       <c r="D57">
-        <v>1922.051790123456</v>
+        <v>1852.19624691358</v>
       </c>
       <c r="E57">
-        <v>5.900403630816742</v>
+        <v>350.4955096588426</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1366,16 +1366,16 @@
         <v>1260.747474747475</v>
       </c>
       <c r="B58">
-        <v>-3885820.167999997</v>
+        <v>-1476176.6298</v>
       </c>
       <c r="C58">
-        <v>-4218.58470065543</v>
+        <v>-1597.948570911151</v>
       </c>
       <c r="D58">
-        <v>1978.515106132027</v>
+        <v>1906.561888297112</v>
       </c>
       <c r="E58">
-        <v>2.743504484554241</v>
+        <v>348.3120683783759</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1383,16 +1383,16 @@
         <v>1277.939393939394</v>
       </c>
       <c r="B59">
-        <v>-4061345.800399996</v>
+        <v>-1542935.300000001</v>
       </c>
       <c r="C59">
-        <v>-4357.00954695429</v>
+        <v>-1650.508450782251</v>
       </c>
       <c r="D59">
-        <v>2035.746883562902</v>
+        <v>1961.666434894399</v>
       </c>
       <c r="E59">
-        <v>-0.4104534472127916</v>
+        <v>346.1231307824887</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1400,16 +1400,16 @@
         <v>1295.131313131313</v>
       </c>
       <c r="B60">
-        <v>-4252664.974999996</v>
+        <v>-1615704.591800001</v>
       </c>
       <c r="C60">
-        <v>-4505.835453876683</v>
+        <v>-1707.021976588858</v>
       </c>
       <c r="D60">
-        <v>2093.74712241608</v>
+        <v>2017.509886705438</v>
       </c>
       <c r="E60">
-        <v>-3.56145565565433</v>
+        <v>343.9287914939852</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1417,16 +1417,16 @@
         <v>1312.323232323232</v>
       </c>
       <c r="B61">
-        <v>-4438590.136399996</v>
+        <v>-1686425.843000001</v>
       </c>
       <c r="C61">
-        <v>-4648.52328366225</v>
+        <v>-1761.208789836603</v>
       </c>
       <c r="D61">
-        <v>2152.515822691562</v>
+        <v>2074.092243730232</v>
       </c>
       <c r="E61">
-        <v>-6.709488017163036</v>
+        <v>341.7291426233481</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1434,16 +1434,16 @@
         <v>1329.515151515152</v>
       </c>
       <c r="B62">
-        <v>-4629668.687999994</v>
+        <v>-1759110.849200001</v>
       </c>
       <c r="C62">
-        <v>-4793.277553447168</v>
+        <v>-1816.184298341801</v>
       </c>
       <c r="D62">
-        <v>2212.052984389348</v>
+        <v>2131.413505968779</v>
       </c>
       <c r="E62">
-        <v>-9.854536778212662</v>
+        <v>339.5242738674877</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1451,16 +1451,16 @@
         <v>1346.707070707071</v>
       </c>
       <c r="B63">
-        <v>-4825967.446599996</v>
+        <v>-1833785.158</v>
       </c>
       <c r="C63">
-        <v>-4940.095688586393</v>
+        <v>-1871.947553644845</v>
       </c>
       <c r="D63">
-        <v>2272.358607509438</v>
+        <v>2189.47367342108</v>
       </c>
       <c r="E63">
-        <v>-12.99658854099996</v>
+        <v>337.3142726033819</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1468,16 +1468,16 @@
         <v>1363.89898989899</v>
       </c>
       <c r="B64">
-        <v>-5027553.228999997</v>
+        <v>-1910474.317</v>
       </c>
       <c r="C64">
-        <v>-5088.975211417082</v>
+        <v>-1928.497643012882</v>
       </c>
       <c r="D64">
-        <v>2333.432692051831</v>
+        <v>2248.272746087134</v>
       </c>
       <c r="E64">
-        <v>-16.13563024981974</v>
+        <v>335.099223976934</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1485,16 +1485,16 @@
         <v>1381.090909090909</v>
       </c>
       <c r="B65">
-        <v>-5246833.927599999</v>
+        <v>-1993899.112</v>
       </c>
       <c r="C65">
-        <v>-5248.856544853877</v>
+        <v>-1989.230854044499</v>
       </c>
       <c r="D65">
-        <v>2395.275238016529</v>
+        <v>2307.810723966942</v>
       </c>
       <c r="E65">
-        <v>-19.27164917812709</v>
+        <v>332.8792109873494</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1502,16 +1502,16 @@
         <v>1398.282828282828</v>
       </c>
       <c r="B66">
-        <v>-5459515.151</v>
+        <v>-2074816.936</v>
       </c>
       <c r="C66">
-        <v>-5401.972687103854</v>
+        <v>-2047.398164672546</v>
       </c>
       <c r="D66">
-        <v>2457.88624540353</v>
+        <v>2368.087607060504</v>
       </c>
       <c r="E66">
-        <v>-22.40463291624398</v>
+        <v>330.6543145673119</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1519,16 +1519,16 @@
         <v>1415.474747474747</v>
       </c>
       <c r="B67">
-        <v>-5677687.779</v>
+        <v>-2157827.755800001</v>
       </c>
       <c r="C67">
-        <v>-5557.143191547533</v>
+        <v>-2106.349721280347</v>
       </c>
       <c r="D67">
-        <v>2521.265714212835</v>
+        <v>2429.103395367819</v>
       </c>
       <c r="E67">
-        <v>-25.53456935967011</v>
+        <v>328.4246136592139</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1536,16 +1536,16 @@
         <v>1432.666666666667</v>
       </c>
       <c r="B68">
-        <v>-5901418.628399999</v>
+        <v>-2242957.119000001</v>
       </c>
       <c r="C68">
-        <v>-5714.365927739591</v>
+        <v>-2166.084739044639</v>
       </c>
       <c r="D68">
-        <v>2585.413644444444</v>
+        <v>2490.858088888888</v>
       </c>
       <c r="E68">
-        <v>-28.66144669796238</v>
+        <v>326.1901852876851</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1553,16 +1553,16 @@
         <v>1449.858585858586</v>
       </c>
       <c r="B69">
-        <v>-6130774.515999997</v>
+        <v>-2330230.573200001</v>
       </c>
       <c r="C69">
-        <v>-5873.638840691533</v>
+        <v>-2226.60246093929</v>
       </c>
       <c r="D69">
-        <v>2650.330036098356</v>
+        <v>2553.351687623711</v>
       </c>
       <c r="E69">
-        <v>-31.78525340414741</v>
+        <v>323.951104628638</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1570,16 +1570,16 @@
         <v>1467.050505050505</v>
       </c>
       <c r="B70">
-        <v>-6379827.279399996</v>
+        <v>-2425003.137000002</v>
       </c>
       <c r="C70">
-        <v>-6044.513167540822</v>
+        <v>-2291.532357802159</v>
       </c>
       <c r="D70">
-        <v>2716.014889174573</v>
+        <v>2616.584191572288</v>
       </c>
       <c r="E70">
-        <v>-34.90597822463724</v>
+        <v>321.7074450750384</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1587,16 +1587,16 @@
         <v>1484.242424242424</v>
       </c>
       <c r="B71">
-        <v>-6620974.519999996</v>
+        <v>-2516771.340200002</v>
       </c>
       <c r="C71">
-        <v>-6208.000864632496</v>
+        <v>-2353.659257175924</v>
       </c>
       <c r="D71">
-        <v>2782.468203673093</v>
+        <v>2680.555600734618</v>
       </c>
       <c r="E71">
-        <v>-38.02361016961672</v>
+        <v>319.459278299593</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1604,16 +1604,16 @@
         <v>1501.434343434343</v>
       </c>
       <c r="B72">
-        <v>-6867951.179599996</v>
+        <v>-2610761.780000002</v>
       </c>
       <c r="C72">
-        <v>-6373.532885256111</v>
+        <v>-2416.56670444097</v>
       </c>
       <c r="D72">
-        <v>2849.689979593919</v>
+        <v>2745.265915110703</v>
       </c>
       <c r="E72">
-        <v>-41.13813850387746</v>
+        <v>317.2066743145315</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1621,16 +1621,16 @@
         <v>1518.626262626263</v>
       </c>
       <c r="B73">
-        <v>-7120824.074999996</v>
+        <v>-2707000.004000001</v>
       </c>
       <c r="C73">
-        <v>-6541.107446584543</v>
+        <v>-2480.254042831226</v>
       </c>
       <c r="D73">
-        <v>2917.680216937047</v>
+        <v>2810.715134700541</v>
       </c>
       <c r="E73">
-        <v>-44.2495527380703</v>
+        <v>314.9497015286513</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1638,16 +1638,16 @@
         <v>1535.818181818182</v>
       </c>
       <c r="B74">
-        <v>-7379660.022999996</v>
+        <v>-2805511.559800001</v>
       </c>
       <c r="C74">
-        <v>-6710.722825376515</v>
+        <v>-2544.720637531127</v>
       </c>
       <c r="D74">
-        <v>2986.438915702479</v>
+        <v>2876.903259504132</v>
       </c>
       <c r="E74">
-        <v>-47.35784262035557</v>
+        <v>312.6884268017776</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1655,16 +1655,16 @@
         <v>1553.010101010101</v>
       </c>
       <c r="B75">
-        <v>-7660295.391999993</v>
+        <v>-2912324.158000001</v>
       </c>
       <c r="C75">
-        <v>-6892.538148907206</v>
+        <v>-2613.82806542986</v>
       </c>
       <c r="D75">
-        <v>3055.966075890215</v>
+        <v>2943.830289521477</v>
       </c>
       <c r="E75">
-        <v>-50.46299812842561</v>
+        <v>310.4229154967856</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1672,16 +1672,16 @@
         <v>1570.20202020202</v>
       </c>
       <c r="B76">
-        <v>-7931618.604999993</v>
+        <v>-3015596.546800001</v>
       </c>
       <c r="C76">
-        <v>-7066.350024446829</v>
+        <v>-2679.897100815116</v>
       </c>
       <c r="D76">
-        <v>3126.261697500255</v>
+        <v>3011.496224752576</v>
       </c>
       <c r="E76">
-        <v>-53.56500946188191</v>
+        <v>308.1532315293184</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1689,16 +1689,16 @@
         <v>1587.393939393939</v>
       </c>
       <c r="B77">
-        <v>-8209109.251399992</v>
+        <v>-3121220.413</v>
       </c>
       <c r="C77">
-        <v>-7242.197789516109</v>
+        <v>-2746.743577135029</v>
       </c>
       <c r="D77">
-        <v>3197.325780532598</v>
+        <v>3079.901065197429</v>
       </c>
       <c r="E77">
-        <v>-56.6638670349451</v>
+        <v>305.8794374153279</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1706,16 +1706,16 @@
         <v>1604.585858585858</v>
       </c>
       <c r="B78">
-        <v>-8492834.147999994</v>
+        <v>-3229221.3042</v>
       </c>
       <c r="C78">
-        <v>-7420.079937210488</v>
+        <v>-2814.366939269154</v>
       </c>
       <c r="D78">
-        <v>3269.158324987245</v>
+        <v>3149.044810856034</v>
       </c>
       <c r="E78">
-        <v>-59.75956146948163</v>
+        <v>303.6015943165552</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1723,16 +1723,16 @@
         <v>1621.777777777778</v>
       </c>
       <c r="B79">
-        <v>-8782860.111599993</v>
+        <v>-3339624.768</v>
       </c>
       <c r="C79">
-        <v>-7599.99500830222</v>
+        <v>-2882.76664966045</v>
       </c>
       <c r="D79">
-        <v>3341.759330864196</v>
+        <v>3218.927461728394</v>
       </c>
       <c r="E79">
-        <v>-62.85208358832859</v>
+        <v>301.319762084062</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1740,16 +1740,16 @@
         <v>1638.969696969697</v>
       </c>
       <c r="B80">
-        <v>-9079253.95899999</v>
+        <v>-3452456.352</v>
       </c>
       <c r="C80">
-        <v>-7781.94158925008</v>
+        <v>-2951.942187582088</v>
       </c>
       <c r="D80">
-        <v>3415.128798163452</v>
+        <v>3289.549017814508</v>
       </c>
       <c r="E80">
-        <v>-65.94142440890235</v>
+        <v>299.0339992999162</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1757,16 +1757,16 @@
         <v>1656.161616161616</v>
       </c>
       <c r="B81">
-        <v>-9400097.767599989</v>
+        <v>-3574600.047000001</v>
       </c>
       <c r="C81">
-        <v>-7976.803664148733</v>
+        <v>-3026.031939439104</v>
       </c>
       <c r="D81">
-        <v>3489.26672688501</v>
+        <v>3360.909479114375</v>
       </c>
       <c r="E81">
-        <v>-69.02757513707458</v>
+        <v>296.7443633171281</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1774,16 +1774,16 @@
         <v>1673.353535353535</v>
       </c>
       <c r="B82">
-        <v>-9709812.355999991</v>
+        <v>-3692511.146000001</v>
       </c>
       <c r="C82">
-        <v>-8162.928499016573</v>
+        <v>-3096.80319766918</v>
       </c>
       <c r="D82">
-        <v>3564.173117028874</v>
+        <v>3433.008845627997</v>
       </c>
       <c r="E82">
-        <v>-72.11052716130347</v>
+        <v>294.4509102979279</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1791,16 +1791,16 @@
         <v>1690.545454545455</v>
       </c>
       <c r="B83">
-        <v>-10026099.20899999</v>
+        <v>-3812928.5108</v>
       </c>
       <c r="C83">
-        <v>-8351.080784326923</v>
+        <v>-3168.348788004103</v>
       </c>
       <c r="D83">
-        <v>3639.847968595041</v>
+        <v>3505.847117355372</v>
       </c>
       <c r="E83">
-        <v>-75.19027204700502</v>
+        <v>292.1536952504704</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1808,16 +1808,16 @@
         <v>1707.737373737374</v>
       </c>
       <c r="B84">
-        <v>-10349025.14339999</v>
+        <v>-3935877.689000001</v>
       </c>
       <c r="C84">
-        <v>-8541.25927357305</v>
+        <v>-3240.66825124998</v>
       </c>
       <c r="D84">
-        <v>3716.291281583512</v>
+        <v>3579.4242942965</v>
       </c>
       <c r="E84">
-        <v>-78.26680153115483</v>
+        <v>289.8527720640467</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1825,16 +1825,16 @@
         <v>1724.929292929293</v>
       </c>
       <c r="B85">
-        <v>-10678656.97599999</v>
+        <v>-4061384.2282</v>
       </c>
       <c r="C85">
-        <v>-8733.462757317575</v>
+        <v>-3313.761141868697</v>
       </c>
       <c r="D85">
-        <v>3793.503055994286</v>
+        <v>3653.740376451382</v>
       </c>
       <c r="E85">
-        <v>-81.34010751710562</v>
+        <v>287.5481935428771</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1842,16 +1842,16 @@
         <v>1742.121212121212</v>
       </c>
       <c r="B86">
-        <v>-11035062.36939999</v>
+        <v>-4197089.332</v>
       </c>
       <c r="C86">
-        <v>-8939.178198325208</v>
+        <v>-3391.996143007525</v>
       </c>
       <c r="D86">
-        <v>3871.483291827364</v>
+        <v>3728.795363820018</v>
       </c>
       <c r="E86">
-        <v>-84.41018206961282</v>
+        <v>285.2400114385576</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1859,16 +1859,16 @@
         <v>1759.313131313131</v>
       </c>
       <c r="B87">
-        <v>-11378710.85499999</v>
+        <v>-4327941.4702</v>
       </c>
       <c r="C87">
-        <v>-9135.547130286119</v>
+        <v>-3466.680036510586</v>
       </c>
       <c r="D87">
-        <v>3950.231989082746</v>
+        <v>3804.589256402407</v>
       </c>
       <c r="E87">
-        <v>-87.47701741005537</v>
+        <v>282.9282764812247</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1876,16 +1876,16 @@
         <v>1776.50505050505</v>
       </c>
       <c r="B88">
-        <v>-11729269.61959999</v>
+        <v>-4461429.115000001</v>
       </c>
       <c r="C88">
-        <v>-9333.937572543438</v>
+        <v>-3542.136073860103</v>
       </c>
       <c r="D88">
-        <v>4029.749147760432</v>
+        <v>3881.122054198551</v>
       </c>
       <c r="E88">
-        <v>-90.54060591184435</v>
+        <v>280.6130384095024</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1893,16 +1893,16 @@
         <v>1793.69696969697</v>
       </c>
       <c r="B89">
-        <v>-12086805.47999999</v>
+        <v>-4597577.814000001</v>
       </c>
       <c r="C89">
-        <v>-9534.348451894359</v>
+        <v>-3618.363859704679</v>
       </c>
       <c r="D89">
-        <v>4110.034767860421</v>
+        <v>3958.393757208447</v>
       </c>
       <c r="E89">
-        <v>-93.60094009600849</v>
+        <v>278.2943459992899</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1910,16 +1910,16 @@
         <v>1810.888888888889</v>
       </c>
       <c r="B90">
-        <v>-12451385.25299999</v>
+        <v>-4736413.114800001</v>
       </c>
       <c r="C90">
-        <v>-9736.778725527513</v>
+        <v>-3695.36300988866</v>
       </c>
       <c r="D90">
-        <v>4191.088849382715</v>
+        <v>4036.404365432098</v>
       </c>
       <c r="E90">
-        <v>-96.65801262694963</v>
+        <v>275.9722470914451</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1927,16 +1927,16 @@
         <v>1828.080808080808</v>
       </c>
       <c r="B91">
-        <v>-12845162.772</v>
+        <v>-4886371.892999999</v>
       </c>
       <c r="C91">
-        <v>-9953.316606268219</v>
+        <v>-3777.731867508444</v>
       </c>
       <c r="D91">
-        <v>4272.911392327312</v>
+        <v>4115.153878869502</v>
       </c>
       <c r="E91">
-        <v>-99.71181630835878</v>
+        <v>273.6467886184174</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1944,16 +1944,16 @@
         <v>1845.272727272727</v>
       </c>
       <c r="B92">
-        <v>-13224455.11</v>
+        <v>-5030818.876799999</v>
       </c>
       <c r="C92">
-        <v>-10159.9012961785</v>
+        <v>-3856.317956580151</v>
       </c>
       <c r="D92">
-        <v>4355.502396694213</v>
+        <v>4194.64229752066</v>
       </c>
       <c r="E92">
-        <v>-102.7623440792865</v>
+        <v>271.3180166298781</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1961,16 +1961,16 @@
         <v>1862.464646464646</v>
       </c>
       <c r="B93">
-        <v>-13610995.7414</v>
+        <v>-5178030.607999998</v>
       </c>
       <c r="C93">
-        <v>-10368.5023676341</v>
+        <v>-3935.674300145354</v>
       </c>
       <c r="D93">
-        <v>4438.861862483419</v>
+        <v>4274.869621385573</v>
       </c>
       <c r="E93">
-        <v>-105.8095890103588</v>
+        <v>268.9859763173953</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1978,16 +1978,16 @@
         <v>1879.656565656566</v>
       </c>
       <c r="B94">
-        <v>-14004851.483</v>
+        <v>-5328032.634199997</v>
       </c>
       <c r="C94">
-        <v>-10579.11889004212</v>
+        <v>-4015.800555387958</v>
       </c>
       <c r="D94">
-        <v>4522.989789694929</v>
+        <v>4355.835850464238</v>
       </c>
       <c r="E94">
-        <v>-108.853544300134</v>
+        <v>266.6507120381986</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -1995,16 +1995,16 @@
         <v>1896.848484848485</v>
       </c>
       <c r="B95">
-        <v>-14406089.1516</v>
+        <v>-5480850.502999999</v>
       </c>
       <c r="C95">
-        <v>-10791.74995796153</v>
+        <v>-4096.69638875742</v>
       </c>
       <c r="D95">
-        <v>4607.886178328742</v>
+        <v>4437.540984756657</v>
       </c>
       <c r="E95">
-        <v>-111.8942032715915</v>
+        <v>264.3122673380735</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2012,16 +2012,16 @@
         <v>1914.040404040404</v>
       </c>
       <c r="B96">
-        <v>-14839049.337</v>
+        <v>-5645755.2212</v>
       </c>
       <c r="C96">
-        <v>-11019.0835417469</v>
+        <v>-4183.189253473684</v>
       </c>
       <c r="D96">
-        <v>4693.551028384858</v>
+        <v>4519.98502426283</v>
       </c>
       <c r="E96">
-        <v>-114.9315593687492</v>
+        <v>261.9706849734262</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2029,16 +2029,16 @@
         <v>1931.232323232323</v>
       </c>
       <c r="B97">
-        <v>-15255695.4826</v>
+        <v>-5804450.856999999</v>
       </c>
       <c r="C97">
-        <v>-11235.85945467894</v>
+        <v>-4265.668499824355</v>
       </c>
       <c r="D97">
-        <v>4779.984339863278</v>
+        <v>4603.167968982756</v>
       </c>
       <c r="E97">
-        <v>-117.9656061534012</v>
+        <v>259.6260069325546</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2046,16 +2046,16 @@
         <v>1948.424242424242</v>
       </c>
       <c r="B98">
-        <v>-15679927.936</v>
+        <v>-5966040.480999998</v>
       </c>
       <c r="C98">
-        <v>-11454.64729047942</v>
+        <v>-4348.916358160588</v>
       </c>
       <c r="D98">
-        <v>4867.186112764002</v>
+        <v>4687.089818916435</v>
       </c>
       <c r="E98">
-        <v>-120.9963373019729</v>
+        <v>257.2782744561636</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2063,16 +2063,16 @@
         <v>1965.616161616161</v>
       </c>
       <c r="B99">
-        <v>-16111813.514</v>
+        <v>-6130549.640799996</v>
       </c>
       <c r="C99">
-        <v>-11675.44623697672</v>
+        <v>-4432.932529290862</v>
       </c>
       <c r="D99">
-        <v>4955.156347087031</v>
+        <v>4771.75057406387</v>
       </c>
       <c r="E99">
-        <v>-124.023746602486</v>
+        <v>254.927528057155</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2080,16 +2080,16 @@
         <v>1982.808080808081</v>
       </c>
       <c r="B100">
-        <v>-16551419.0334</v>
+        <v>-6298003.883999996</v>
       </c>
       <c r="C100">
-        <v>-11898.25550299354</v>
+        <v>-4517.716721757636</v>
       </c>
       <c r="D100">
-        <v>5043.895042832362</v>
+        <v>4857.150234425058</v>
       </c>
       <c r="E100">
-        <v>-127.0478279516304</v>
+        <v>252.573807539725</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2097,16 +2097,16 @@
         <v>2000</v>
       </c>
       <c r="B101">
-        <v>-17025372.426</v>
+        <v>-6478546.807799997</v>
       </c>
       <c r="C101">
-        <v>-12136.36151873002</v>
+        <v>-4608.32502085771</v>
       </c>
       <c r="D101">
-        <v>5133.4022</v>
+        <v>4943.2888</v>
       </c>
       <c r="E101">
-        <v>-130.0685753519375</v>
+        <v>250.2171520177995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>